<commit_message>
changed name of some samples, hyphen issue
</commit_message>
<xml_diff>
--- a/data/met.xlsx
+++ b/data/met.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspkaur\Google Drive\Metagenomics\pico_comb_run\pico\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64E4E3D-503A-4D94-AE2E-3AF26891A404}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4217ABF8-D6CD-4C66-B574-E989EAA1A8D7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1741" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1741" uniqueCount="434">
   <si>
     <t>Year</t>
   </si>
@@ -1189,12 +1189,6 @@
     <t>NC-soil</t>
   </si>
   <si>
-    <t>p12-3</t>
-  </si>
-  <si>
-    <t>p12-4</t>
-  </si>
-  <si>
     <t>OM</t>
   </si>
   <si>
@@ -1303,22 +1297,40 @@
     <t>S_SALTS</t>
   </si>
   <si>
-    <t>conps1-1</t>
-  </si>
-  <si>
-    <t>conps1-2</t>
-  </si>
-  <si>
-    <t>conps1-4</t>
-  </si>
-  <si>
-    <t>conps1-5</t>
-  </si>
-  <si>
-    <t>conps1-10</t>
-  </si>
-  <si>
-    <t>conps1-11</t>
+    <t>NC.root</t>
+  </si>
+  <si>
+    <t>PC.root</t>
+  </si>
+  <si>
+    <t>PC.soil</t>
+  </si>
+  <si>
+    <t>NC.soil</t>
+  </si>
+  <si>
+    <t>p12.3</t>
+  </si>
+  <si>
+    <t>p12.4</t>
+  </si>
+  <si>
+    <t>conps1.1</t>
+  </si>
+  <si>
+    <t>conps1.2</t>
+  </si>
+  <si>
+    <t>conps1.4</t>
+  </si>
+  <si>
+    <t>conps1.5</t>
+  </si>
+  <si>
+    <t>conps1.10</t>
+  </si>
+  <si>
+    <t>conps1.11</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1820,7 @@
       <pane xSplit="10" ySplit="20" topLeftCell="AE363" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="AM27" sqref="AM27"/>
+      <selection pane="bottomRight" activeCell="H375" sqref="H375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,94 +1851,94 @@
         <v>380</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>394</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>395</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>397</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>399</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>401</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="W1" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y1" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Z1" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>404</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AB1" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="AC1" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="AB1" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AE1" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AF1" s="19" t="s">
         <v>408</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AG1" s="38" t="s">
         <v>409</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AH1" s="20" t="s">
         <v>410</v>
       </c>
-      <c r="AG1" s="38" t="s">
+      <c r="AI1" s="21" t="s">
         <v>411</v>
       </c>
-      <c r="AH1" s="20" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>412</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
         <v>413</v>
-      </c>
-      <c r="AJ1" s="21" t="s">
-        <v>414</v>
-      </c>
-      <c r="AK1" s="21" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
@@ -2042,7 +2054,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>382</v>
+        <v>422</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>382</v>
@@ -2993,7 +3005,7 @@
         <v>186</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>6</v>
@@ -3104,7 +3116,7 @@
         <v>186</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>6</v>
@@ -3215,7 +3227,7 @@
         <v>186</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>6</v>
@@ -3326,7 +3338,7 @@
         <v>186</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>6</v>
@@ -6164,7 +6176,7 @@
         <v>186</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>6</v>
@@ -6275,7 +6287,7 @@
         <v>186</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>6</v>
@@ -6386,7 +6398,7 @@
         <v>186</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>6</v>
@@ -6497,7 +6509,7 @@
         <v>186</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>6</v>
@@ -6608,7 +6620,7 @@
         <v>186</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>6</v>
@@ -6715,7 +6727,7 @@
         <v>186</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>6</v>
@@ -6822,7 +6834,7 @@
         <v>186</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>6</v>
@@ -6929,7 +6941,7 @@
         <v>186</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>6</v>
@@ -9315,7 +9327,7 @@
     </row>
     <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>383</v>
+        <v>423</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>383</v>
@@ -9378,7 +9390,7 @@
         <v>186</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>6</v>
@@ -9477,7 +9489,7 @@
         <v>186</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>6</v>
@@ -10611,7 +10623,7 @@
         <v>186</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>6</v>
@@ -10722,7 +10734,7 @@
         <v>5</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>6</v>
@@ -10829,7 +10841,7 @@
         <v>186</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>6</v>
@@ -10936,7 +10948,7 @@
         <v>186</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>6</v>
@@ -11043,7 +11055,7 @@
         <v>5</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>6</v>
@@ -11142,7 +11154,7 @@
         <v>5</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>6</v>
@@ -11241,7 +11253,7 @@
         <v>5</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>6</v>
@@ -11340,7 +11352,7 @@
         <v>186</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>6</v>
@@ -11439,7 +11451,7 @@
         <v>186</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>6</v>
@@ -11538,7 +11550,7 @@
         <v>186</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>6</v>
@@ -12636,7 +12648,7 @@
         <v>186</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>6</v>
@@ -12747,7 +12759,7 @@
         <v>186</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>6</v>
@@ -12858,7 +12870,7 @@
         <v>186</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>6</v>
@@ -12969,7 +12981,7 @@
         <v>186</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>6</v>
@@ -16025,7 +16037,7 @@
         <v>186</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>6</v>
@@ -16136,7 +16148,7 @@
         <v>186</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>6</v>
@@ -16247,7 +16259,7 @@
         <v>186</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>6</v>
@@ -16358,7 +16370,7 @@
         <v>186</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>6</v>
@@ -16469,7 +16481,7 @@
         <v>186</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>6</v>
@@ -16576,7 +16588,7 @@
         <v>186</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>6</v>
@@ -16683,7 +16695,7 @@
         <v>186</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>6</v>
@@ -16790,7 +16802,7 @@
         <v>186</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>6</v>
@@ -19744,7 +19756,7 @@
         <v>186</v>
       </c>
       <c r="E177" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>6</v>
@@ -19856,7 +19868,7 @@
         <v>186</v>
       </c>
       <c r="E178" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F178" s="2" t="s">
         <v>6</v>
@@ -19968,7 +19980,7 @@
         <v>186</v>
       </c>
       <c r="E179" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>6</v>
@@ -20080,7 +20092,7 @@
         <v>186</v>
       </c>
       <c r="E180" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F180" s="2" t="s">
         <v>6</v>
@@ -20192,7 +20204,7 @@
         <v>186</v>
       </c>
       <c r="E181" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>6</v>
@@ -20304,7 +20316,7 @@
         <v>186</v>
       </c>
       <c r="E182" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>6</v>
@@ -20416,7 +20428,7 @@
         <v>186</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>6</v>
@@ -20528,7 +20540,7 @@
         <v>186</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F184" s="2" t="s">
         <v>6</v>
@@ -20640,7 +20652,7 @@
         <v>186</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F185" s="2" t="s">
         <v>6</v>
@@ -20752,7 +20764,7 @@
         <v>5</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F186" s="2" t="s">
         <v>6</v>
@@ -20859,7 +20871,7 @@
         <v>186</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F187" s="2" t="s">
         <v>6</v>
@@ -20966,7 +20978,7 @@
         <v>186</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F188" s="2" t="s">
         <v>6</v>
@@ -21073,7 +21085,7 @@
         <v>186</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F189" s="2" t="s">
         <v>6</v>
@@ -21180,7 +21192,7 @@
         <v>5</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F190" s="2" t="s">
         <v>6</v>
@@ -21279,7 +21291,7 @@
         <v>5</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F191" s="2" t="s">
         <v>6</v>
@@ -21378,7 +21390,7 @@
         <v>186</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F192" s="2" t="s">
         <v>6</v>
@@ -21477,7 +21489,7 @@
         <v>186</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F193" s="2" t="s">
         <v>6</v>
@@ -21576,7 +21588,7 @@
         <v>186</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F194" s="2" t="s">
         <v>6</v>
@@ -21675,7 +21687,7 @@
         <v>186</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F195" s="2" t="s">
         <v>6</v>
@@ -21774,7 +21786,7 @@
         <v>186</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F196" s="2" t="s">
         <v>6</v>
@@ -22759,7 +22771,7 @@
       </c>
       <c r="D205" s="3"/>
       <c r="E205" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F205" s="3" t="s">
         <v>1</v>
@@ -22870,7 +22882,7 @@
       </c>
       <c r="D206" s="3"/>
       <c r="E206" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F206" s="3" t="s">
         <v>1</v>
@@ -22981,7 +22993,7 @@
       </c>
       <c r="D207" s="3"/>
       <c r="E207" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F207" s="3" t="s">
         <v>1</v>
@@ -23092,7 +23104,7 @@
       </c>
       <c r="D208" s="3"/>
       <c r="E208" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F208" s="3" t="s">
         <v>1</v>
@@ -23203,7 +23215,7 @@
       </c>
       <c r="D209" s="3"/>
       <c r="E209" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F209" s="3" t="s">
         <v>1</v>
@@ -24630,7 +24642,7 @@
       </c>
       <c r="D222" s="3"/>
       <c r="E222" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>1</v>
@@ -24741,7 +24753,7 @@
       </c>
       <c r="D223" s="3"/>
       <c r="E223" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>1</v>
@@ -24852,7 +24864,7 @@
       </c>
       <c r="D224" s="3"/>
       <c r="E224" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F224" s="3" t="s">
         <v>1</v>
@@ -24963,7 +24975,7 @@
       </c>
       <c r="D225" s="3"/>
       <c r="E225" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F225" s="3" t="s">
         <v>1</v>
@@ -25074,7 +25086,7 @@
       </c>
       <c r="D226" s="3"/>
       <c r="E226" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F226" s="3" t="s">
         <v>1</v>
@@ -25185,7 +25197,7 @@
       </c>
       <c r="D227" s="3"/>
       <c r="E227" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F227" s="3" t="s">
         <v>1</v>
@@ -25296,7 +25308,7 @@
       </c>
       <c r="D228" s="3"/>
       <c r="E228" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F228" s="3" t="s">
         <v>1</v>
@@ -25403,7 +25415,7 @@
       </c>
       <c r="D229" s="3"/>
       <c r="E229" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F229" s="3" t="s">
         <v>1</v>
@@ -25510,7 +25522,7 @@
       </c>
       <c r="D230" s="3"/>
       <c r="E230" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F230" s="3" t="s">
         <v>1</v>
@@ -25617,7 +25629,7 @@
       </c>
       <c r="D231" s="3"/>
       <c r="E231" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F231" s="3" t="s">
         <v>1</v>
@@ -25724,7 +25736,7 @@
       </c>
       <c r="D232" s="3"/>
       <c r="E232" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F232" s="3" t="s">
         <v>1</v>
@@ -25823,7 +25835,7 @@
       </c>
       <c r="D233" s="3"/>
       <c r="E233" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F233" s="3" t="s">
         <v>1</v>
@@ -25922,7 +25934,7 @@
       </c>
       <c r="D234" s="3"/>
       <c r="E234" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F234" s="3" t="s">
         <v>1</v>
@@ -26021,7 +26033,7 @@
       </c>
       <c r="D235" s="3"/>
       <c r="E235" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F235" s="3" t="s">
         <v>1</v>
@@ -28786,7 +28798,7 @@
       </c>
       <c r="D262" s="3"/>
       <c r="E262" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F262" s="3" t="s">
         <v>1</v>
@@ -28898,7 +28910,7 @@
       </c>
       <c r="D263" s="3"/>
       <c r="E263" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F263" s="3" t="s">
         <v>1</v>
@@ -29010,7 +29022,7 @@
       </c>
       <c r="D264" s="3"/>
       <c r="E264" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F264" s="3" t="s">
         <v>1</v>
@@ -29122,7 +29134,7 @@
       </c>
       <c r="D265" s="3"/>
       <c r="E265" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F265" s="3" t="s">
         <v>1</v>
@@ -29234,7 +29246,7 @@
       </c>
       <c r="D266" s="3"/>
       <c r="E266" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F266" s="3" t="s">
         <v>1</v>
@@ -29345,7 +29357,7 @@
       </c>
       <c r="D267" s="3"/>
       <c r="E267" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F267" s="3" t="s">
         <v>1</v>
@@ -29456,7 +29468,7 @@
       </c>
       <c r="D268" s="3"/>
       <c r="E268" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F268" s="3" t="s">
         <v>1</v>
@@ -29563,7 +29575,7 @@
       </c>
       <c r="D269" s="3"/>
       <c r="E269" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F269" s="3" t="s">
         <v>1</v>
@@ -29670,7 +29682,7 @@
       </c>
       <c r="D270" s="3"/>
       <c r="E270" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F270" s="3" t="s">
         <v>1</v>
@@ -29769,7 +29781,7 @@
       </c>
       <c r="D271" s="3"/>
       <c r="E271" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F271" s="3" t="s">
         <v>1</v>
@@ -29868,7 +29880,7 @@
       </c>
       <c r="D272" s="3"/>
       <c r="E272" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F272" s="3" t="s">
         <v>1</v>
@@ -29967,7 +29979,7 @@
       </c>
       <c r="D273" s="3"/>
       <c r="E273" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F273" s="3" t="s">
         <v>1</v>
@@ -30066,7 +30078,7 @@
       </c>
       <c r="D274" s="3"/>
       <c r="E274" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F274" s="3" t="s">
         <v>1</v>
@@ -30165,7 +30177,7 @@
       </c>
       <c r="D275" s="3"/>
       <c r="E275" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F275" s="3" t="s">
         <v>1</v>
@@ -30264,7 +30276,7 @@
       </c>
       <c r="D276" s="3"/>
       <c r="E276" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F276" s="3" t="s">
         <v>1</v>
@@ -30375,7 +30387,7 @@
       </c>
       <c r="D277" s="3"/>
       <c r="E277" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F277" s="3" t="s">
         <v>1</v>
@@ -30476,7 +30488,7 @@
     </row>
     <row r="278" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A278" s="5" t="s">
-        <v>384</v>
+        <v>424</v>
       </c>
       <c r="B278" s="5" t="s">
         <v>384</v>
@@ -30527,7 +30539,7 @@
     </row>
     <row r="279" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A279" s="5" t="s">
-        <v>385</v>
+        <v>425</v>
       </c>
       <c r="B279" s="5" t="s">
         <v>385</v>
@@ -30588,7 +30600,7 @@
       </c>
       <c r="D280" s="9"/>
       <c r="E280" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F280" s="3" t="s">
         <v>1</v>
@@ -30699,7 +30711,7 @@
       </c>
       <c r="D281" s="9"/>
       <c r="E281" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F281" s="3" t="s">
         <v>1</v>
@@ -31244,7 +31256,7 @@
     </row>
     <row r="286" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A286" s="7" t="s">
-        <v>386</v>
+        <v>426</v>
       </c>
       <c r="B286" s="9">
         <v>2015</v>
@@ -31355,7 +31367,7 @@
     </row>
     <row r="287" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A287" s="7" t="s">
-        <v>387</v>
+        <v>427</v>
       </c>
       <c r="B287" s="9">
         <v>2015</v>
@@ -31476,7 +31488,7 @@
       </c>
       <c r="D288" s="9"/>
       <c r="E288" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F288" s="3" t="s">
         <v>1</v>
@@ -31587,7 +31599,7 @@
       </c>
       <c r="D289" s="9"/>
       <c r="E289" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F289" s="3" t="s">
         <v>1</v>
@@ -31698,7 +31710,7 @@
       </c>
       <c r="D290" s="9"/>
       <c r="E290" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F290" s="3" t="s">
         <v>1</v>
@@ -31809,7 +31821,7 @@
       </c>
       <c r="D291" s="9"/>
       <c r="E291" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F291" s="3" t="s">
         <v>1</v>
@@ -31920,7 +31932,7 @@
       </c>
       <c r="D292" s="9"/>
       <c r="E292" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F292" s="3" t="s">
         <v>1</v>
@@ -32031,7 +32043,7 @@
       </c>
       <c r="D293" s="9"/>
       <c r="E293" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F293" s="3" t="s">
         <v>1</v>
@@ -32142,7 +32154,7 @@
       </c>
       <c r="D294" s="9"/>
       <c r="E294" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F294" s="3" t="s">
         <v>1</v>
@@ -32253,7 +32265,7 @@
       </c>
       <c r="D295" s="9"/>
       <c r="E295" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F295" s="3" t="s">
         <v>1</v>
@@ -33458,7 +33470,7 @@
       </c>
       <c r="D306" s="9"/>
       <c r="E306" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F306" s="3" t="s">
         <v>1</v>
@@ -33569,7 +33581,7 @@
       </c>
       <c r="D307" s="9"/>
       <c r="E307" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F307" s="3" t="s">
         <v>1</v>
@@ -33680,7 +33692,7 @@
       </c>
       <c r="D308" s="9"/>
       <c r="E308" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F308" s="3" t="s">
         <v>1</v>
@@ -33791,7 +33803,7 @@
       </c>
       <c r="D309" s="9"/>
       <c r="E309" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F309" s="3" t="s">
         <v>1</v>
@@ -33902,7 +33914,7 @@
       </c>
       <c r="D310" s="9"/>
       <c r="E310" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F310" s="3" t="s">
         <v>1</v>
@@ -34013,7 +34025,7 @@
       </c>
       <c r="D311" s="9"/>
       <c r="E311" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F311" s="3" t="s">
         <v>1</v>
@@ -34124,7 +34136,7 @@
       </c>
       <c r="D312" s="9"/>
       <c r="E312" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F312" s="3" t="s">
         <v>1</v>
@@ -34235,7 +34247,7 @@
       </c>
       <c r="D313" s="9"/>
       <c r="E313" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F313" s="3" t="s">
         <v>1</v>
@@ -34346,7 +34358,7 @@
       </c>
       <c r="D314" s="9"/>
       <c r="E314" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F314" s="3" t="s">
         <v>1</v>
@@ -34453,7 +34465,7 @@
       </c>
       <c r="D315" s="9"/>
       <c r="E315" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F315" s="3" t="s">
         <v>1</v>
@@ -34560,7 +34572,7 @@
       </c>
       <c r="D316" s="9"/>
       <c r="E316" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F316" s="3" t="s">
         <v>1</v>
@@ -34667,7 +34679,7 @@
       </c>
       <c r="D317" s="9"/>
       <c r="E317" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F317" s="3" t="s">
         <v>1</v>
@@ -34774,7 +34786,7 @@
       </c>
       <c r="D318" s="9"/>
       <c r="E318" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F318" s="3" t="s">
         <v>1</v>
@@ -34873,7 +34885,7 @@
       </c>
       <c r="D319" s="9"/>
       <c r="E319" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F319" s="3" t="s">
         <v>1</v>
@@ -34972,7 +34984,7 @@
       </c>
       <c r="D320" s="9"/>
       <c r="E320" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F320" s="3" t="s">
         <v>1</v>
@@ -35071,7 +35083,7 @@
       </c>
       <c r="D321" s="9"/>
       <c r="E321" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F321" s="3" t="s">
         <v>1</v>
@@ -35170,7 +35182,7 @@
       </c>
       <c r="D322" s="9"/>
       <c r="E322" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F322" s="3" t="s">
         <v>1</v>
@@ -35269,7 +35281,7 @@
       </c>
       <c r="D323" s="9"/>
       <c r="E323" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F323" s="3" t="s">
         <v>1</v>
@@ -37872,7 +37884,7 @@
       </c>
       <c r="D348" s="9"/>
       <c r="E348" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F348" s="3" t="s">
         <v>1</v>
@@ -37984,7 +37996,7 @@
       </c>
       <c r="D349" s="9"/>
       <c r="E349" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F349" s="3" t="s">
         <v>1</v>
@@ -38096,7 +38108,7 @@
       </c>
       <c r="D350" s="9"/>
       <c r="E350" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F350" s="3" t="s">
         <v>1</v>
@@ -38208,7 +38220,7 @@
       </c>
       <c r="D351" s="9"/>
       <c r="E351" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F351" s="3" t="s">
         <v>1</v>
@@ -38320,7 +38332,7 @@
       </c>
       <c r="D352" s="9"/>
       <c r="E352" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F352" s="3" t="s">
         <v>1</v>
@@ -38432,7 +38444,7 @@
       </c>
       <c r="D353" s="9"/>
       <c r="E353" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F353" s="3" t="s">
         <v>1</v>
@@ -38544,7 +38556,7 @@
       </c>
       <c r="D354" s="9"/>
       <c r="E354" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F354" s="3" t="s">
         <v>1</v>
@@ -38655,7 +38667,7 @@
       </c>
       <c r="D355" s="9"/>
       <c r="E355" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F355" s="3" t="s">
         <v>1</v>
@@ -38766,7 +38778,7 @@
       </c>
       <c r="D356" s="9"/>
       <c r="E356" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F356" s="3" t="s">
         <v>1</v>
@@ -38873,7 +38885,7 @@
       </c>
       <c r="D357" s="9"/>
       <c r="E357" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F357" s="3" t="s">
         <v>1</v>
@@ -38980,7 +38992,7 @@
       </c>
       <c r="D358" s="9"/>
       <c r="E358" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F358" s="3" t="s">
         <v>1</v>
@@ -39079,7 +39091,7 @@
       </c>
       <c r="D359" s="9"/>
       <c r="E359" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F359" s="3" t="s">
         <v>1</v>
@@ -39178,7 +39190,7 @@
       </c>
       <c r="D360" s="9"/>
       <c r="E360" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F360" s="3" t="s">
         <v>1</v>
@@ -39277,7 +39289,7 @@
       </c>
       <c r="D361" s="9"/>
       <c r="E361" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F361" s="3" t="s">
         <v>1</v>
@@ -39376,7 +39388,7 @@
       </c>
       <c r="D362" s="9"/>
       <c r="E362" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F362" s="3" t="s">
         <v>1</v>
@@ -39475,7 +39487,7 @@
       </c>
       <c r="D363" s="9"/>
       <c r="E363" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F363" s="3" t="s">
         <v>1</v>
@@ -39574,7 +39586,7 @@
       </c>
       <c r="D364" s="9"/>
       <c r="E364" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F364" s="3" t="s">
         <v>1</v>
@@ -39673,7 +39685,7 @@
       </c>
       <c r="D365" s="9"/>
       <c r="E365" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F365" s="3" t="s">
         <v>1</v>
@@ -39772,7 +39784,7 @@
       </c>
       <c r="D366" s="9"/>
       <c r="E366" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F366" s="3" t="s">
         <v>1</v>
@@ -39883,7 +39895,7 @@
       </c>
       <c r="D367" s="9"/>
       <c r="E367" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F367" s="3" t="s">
         <v>1</v>
@@ -39984,7 +39996,7 @@
     </row>
     <row r="368" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A368" s="7" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="B368" s="9">
         <v>2015</v>
@@ -40010,7 +40022,7 @@
     </row>
     <row r="369" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A369" s="7" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="B369" s="9">
         <v>2015</v>
@@ -40036,7 +40048,7 @@
     </row>
     <row r="370" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A370" s="7" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B370" s="9">
         <v>2016</v>
@@ -40074,7 +40086,7 @@
     </row>
     <row r="371" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A371" s="7" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B371" s="9">
         <v>2016</v>
@@ -40112,7 +40124,7 @@
     </row>
     <row r="372" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A372" s="7" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B372" s="9">
         <v>2017</v>
@@ -40150,7 +40162,7 @@
     </row>
     <row r="373" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A373" s="7" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="B373" s="9">
         <v>2017</v>
@@ -40219,7 +40231,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B2" s="2">
         <v>2015</v>
@@ -40230,7 +40242,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B3" s="4">
         <v>2016</v>
@@ -40241,7 +40253,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B4" s="2">
         <v>2017</v>
@@ -40252,7 +40264,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B5" s="2">
         <v>2015</v>
@@ -40263,7 +40275,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B6" s="4">
         <v>2016</v>
@@ -40274,7 +40286,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B7" s="2">
         <v>2017</v>

</xml_diff>

<commit_message>
corrected errors in met file
</commit_message>
<xml_diff>
--- a/data/met.xlsx
+++ b/data/met.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspkaur\Google Drive\Metagenomics\pico_comb_run\pico\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFACAEF3-3737-49E8-AF1C-733EEA85784D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42072BBE-276A-4EC9-A53B-DD03A5C114A5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="11730" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="with_just_pg_envt" sheetId="13" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">envt_comp!$C$1:$C$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$A$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">with_just_pg_envt!$B$1:$C$373</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">with_just_pg_envt!$F$1:$F$373</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1920,13 +1920,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AN373"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="20" topLeftCell="M359" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="12" ySplit="20" topLeftCell="M350" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="G281" sqref="G281"/>
+      <selection pane="bottomRight" activeCell="K369" sqref="K369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2057,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>422</v>
       </c>
@@ -2226,7 +2227,7 @@
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2343,7 +2344,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2460,7 +2461,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2694,7 +2695,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2811,7 +2812,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -3045,7 +3046,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>0.106641366223909</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -3279,7 +3280,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -3396,7 +3397,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -3513,7 +3514,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -3630,7 +3631,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3747,7 +3748,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3864,7 +3865,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -3981,7 +3982,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -4098,7 +4099,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -4215,7 +4216,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -4332,7 +4333,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -4449,7 +4450,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -4566,7 +4567,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -4683,7 +4684,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -4800,7 +4801,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -4917,7 +4918,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -5034,7 +5035,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -5151,7 +5152,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -5264,7 +5265,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -5490,7 +5491,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -5603,7 +5604,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -5716,7 +5717,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -5829,7 +5830,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -5942,7 +5943,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -6055,7 +6056,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -6168,7 +6169,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -6281,7 +6282,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -6394,7 +6395,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -6507,7 +6508,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
@@ -6624,7 +6625,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -6741,7 +6742,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
@@ -6858,7 +6859,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -6975,7 +6976,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
@@ -7088,7 +7089,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
@@ -7201,7 +7202,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -7314,7 +7315,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -7427,7 +7428,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -7544,7 +7545,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -7661,7 +7662,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -7778,7 +7779,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -7895,7 +7896,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -8012,7 +8013,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
@@ -8129,7 +8130,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
@@ -8246,7 +8247,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
@@ -8363,7 +8364,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>61</v>
       </c>
@@ -8480,7 +8481,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>62</v>
       </c>
@@ -8597,7 +8598,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
@@ -8714,7 +8715,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
@@ -8827,7 +8828,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>65</v>
       </c>
@@ -8940,7 +8941,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
@@ -9053,7 +9054,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
@@ -9166,7 +9167,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>68</v>
       </c>
@@ -9279,7 +9280,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>69</v>
       </c>
@@ -9392,7 +9393,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
@@ -9505,7 +9506,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
@@ -9618,7 +9619,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
@@ -9731,7 +9732,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
@@ -9844,7 +9845,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>423</v>
       </c>
@@ -9897,7 +9898,7 @@
       <c r="AL70" s="2"/>
       <c r="AM70" s="2"/>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>181</v>
       </c>
@@ -10002,7 +10003,7 @@
       <c r="AL71" s="3"/>
       <c r="AM71" s="3"/>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>182</v>
       </c>
@@ -10107,7 +10108,7 @@
       <c r="AL72" s="3"/>
       <c r="AM72" s="3"/>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>183</v>
       </c>
@@ -10212,7 +10213,7 @@
       <c r="AL73" s="3"/>
       <c r="AM73" s="3"/>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>74</v>
       </c>
@@ -10317,7 +10318,7 @@
       <c r="AL74" s="3"/>
       <c r="AM74" s="3"/>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>75</v>
       </c>
@@ -10422,7 +10423,7 @@
       <c r="AL75" s="2"/>
       <c r="AM75" s="2"/>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>76</v>
       </c>
@@ -10527,7 +10528,7 @@
       <c r="AL76" s="2"/>
       <c r="AM76" s="2"/>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>77</v>
       </c>
@@ -10632,7 +10633,7 @@
       <c r="AL77" s="2"/>
       <c r="AM77" s="2"/>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -10683,7 +10684,7 @@
       <c r="AF78" s="2"/>
       <c r="AG78" s="2"/>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>79</v>
       </c>
@@ -10734,7 +10735,7 @@
       <c r="AF79" s="2"/>
       <c r="AG79" s="2"/>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>80</v>
       </c>
@@ -10785,7 +10786,7 @@
       <c r="AF80" s="2"/>
       <c r="AG80" s="2"/>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>81</v>
       </c>
@@ -10836,7 +10837,7 @@
       <c r="AF81" s="2"/>
       <c r="AG81" s="2"/>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>82</v>
       </c>
@@ -10887,7 +10888,7 @@
       <c r="AF82" s="2"/>
       <c r="AG82" s="2"/>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>83</v>
       </c>
@@ -10938,7 +10939,7 @@
       <c r="AF83" s="2"/>
       <c r="AG83" s="2"/>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>84</v>
       </c>
@@ -10989,7 +10990,7 @@
       <c r="AF84" s="2"/>
       <c r="AG84" s="2"/>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>85</v>
       </c>
@@ -11040,7 +11041,7 @@
       <c r="AF85" s="2"/>
       <c r="AG85" s="2"/>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>86</v>
       </c>
@@ -11091,7 +11092,7 @@
       <c r="AF86" s="2"/>
       <c r="AG86" s="2"/>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>87</v>
       </c>
@@ -11142,7 +11143,7 @@
       <c r="AF87" s="2"/>
       <c r="AG87" s="2"/>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>88</v>
       </c>
@@ -11193,7 +11194,7 @@
       <c r="AF88" s="2"/>
       <c r="AG88" s="2"/>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>89</v>
       </c>
@@ -11244,7 +11245,7 @@
       <c r="AF89" s="2"/>
       <c r="AG89" s="2"/>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -11361,7 +11362,7 @@
         <v>6.1917808219178097E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>91</v>
       </c>
@@ -11474,7 +11475,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>92</v>
       </c>
@@ -11587,7 +11588,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>93</v>
       </c>
@@ -11700,7 +11701,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>94</v>
       </c>
@@ -11805,7 +11806,7 @@
       <c r="AL94" s="2"/>
       <c r="AM94" s="2"/>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -11910,7 +11911,7 @@
       <c r="AL95" s="2"/>
       <c r="AM95" s="2"/>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>96</v>
       </c>
@@ -12015,7 +12016,7 @@
       <c r="AL96" s="2"/>
       <c r="AM96" s="2"/>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>97</v>
       </c>
@@ -12120,7 +12121,7 @@
       <c r="AL97" s="2"/>
       <c r="AM97" s="2"/>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>98</v>
       </c>
@@ -12225,7 +12226,7 @@
       <c r="AL98" s="2"/>
       <c r="AM98" s="2"/>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>99</v>
       </c>
@@ -12330,7 +12331,7 @@
       <c r="AL99" s="2"/>
       <c r="AM99" s="2"/>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>199</v>
       </c>
@@ -12447,7 +12448,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>200</v>
       </c>
@@ -12564,7 +12565,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>201</v>
       </c>
@@ -12681,7 +12682,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>202</v>
       </c>
@@ -12798,7 +12799,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>203</v>
       </c>
@@ -12915,7 +12916,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>204</v>
       </c>
@@ -13032,7 +13033,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>205</v>
       </c>
@@ -13149,7 +13150,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>206</v>
       </c>
@@ -13266,7 +13267,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>207</v>
       </c>
@@ -13383,7 +13384,7 @@
         <v>0.106641366223909</v>
       </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>208</v>
       </c>
@@ -13500,7 +13501,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>209</v>
       </c>
@@ -13617,7 +13618,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>210</v>
       </c>
@@ -13734,7 +13735,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>211</v>
       </c>
@@ -13851,7 +13852,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>212</v>
       </c>
@@ -13968,7 +13969,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>213</v>
       </c>
@@ -14085,7 +14086,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>214</v>
       </c>
@@ -14202,7 +14203,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>215</v>
       </c>
@@ -14319,7 +14320,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>216</v>
       </c>
@@ -14436,7 +14437,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>217</v>
       </c>
@@ -14553,7 +14554,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>218</v>
       </c>
@@ -14670,7 +14671,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>219</v>
       </c>
@@ -14787,7 +14788,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>220</v>
       </c>
@@ -14904,7 +14905,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>221</v>
       </c>
@@ -15021,7 +15022,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>222</v>
       </c>
@@ -15138,7 +15139,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>223</v>
       </c>
@@ -15255,7 +15256,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>224</v>
       </c>
@@ -15372,7 +15373,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>225</v>
       </c>
@@ -15489,7 +15490,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>226</v>
       </c>
@@ -15602,7 +15603,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>227</v>
       </c>
@@ -15715,7 +15716,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="129" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>228</v>
       </c>
@@ -15828,7 +15829,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="130" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>229</v>
       </c>
@@ -15941,7 +15942,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="131" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>230</v>
       </c>
@@ -16054,7 +16055,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="132" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>231</v>
       </c>
@@ -16167,7 +16168,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="133" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>232</v>
       </c>
@@ -16280,7 +16281,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="134" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>233</v>
       </c>
@@ -16393,7 +16394,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="135" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>234</v>
       </c>
@@ -16506,7 +16507,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="136" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>235</v>
       </c>
@@ -16619,7 +16620,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="137" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>236</v>
       </c>
@@ -16732,7 +16733,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="138" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>237</v>
       </c>
@@ -16845,7 +16846,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="139" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>238</v>
       </c>
@@ -16958,7 +16959,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="140" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>239</v>
       </c>
@@ -17075,7 +17076,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="141" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>240</v>
       </c>
@@ -17192,7 +17193,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="142" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>241</v>
       </c>
@@ -17309,7 +17310,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="143" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>242</v>
       </c>
@@ -17426,7 +17427,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="144" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>243</v>
       </c>
@@ -17539,7 +17540,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="145" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>244</v>
       </c>
@@ -17652,7 +17653,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="146" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>245</v>
       </c>
@@ -17765,7 +17766,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="147" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>246</v>
       </c>
@@ -17870,7 +17871,7 @@
       <c r="AL147" s="2"/>
       <c r="AM147" s="2"/>
     </row>
-    <row r="148" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>247</v>
       </c>
@@ -17987,7 +17988,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="149" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>248</v>
       </c>
@@ -18104,7 +18105,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="150" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>249</v>
       </c>
@@ -18221,7 +18222,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="151" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>250</v>
       </c>
@@ -18338,7 +18339,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="152" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>251</v>
       </c>
@@ -18455,7 +18456,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="153" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>252</v>
       </c>
@@ -18572,7 +18573,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="154" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>253</v>
       </c>
@@ -18689,7 +18690,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="155" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>254</v>
       </c>
@@ -18806,7 +18807,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="156" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>255</v>
       </c>
@@ -18923,7 +18924,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="157" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>256</v>
       </c>
@@ -19040,7 +19041,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="158" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>257</v>
       </c>
@@ -19153,7 +19154,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="159" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>258</v>
       </c>
@@ -19266,7 +19267,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="160" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
         <v>259</v>
       </c>
@@ -19379,7 +19380,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="161" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
         <v>260</v>
       </c>
@@ -19492,7 +19493,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="162" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
         <v>261</v>
       </c>
@@ -19605,7 +19606,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="163" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
         <v>262</v>
       </c>
@@ -19718,7 +19719,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="164" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
         <v>263</v>
       </c>
@@ -19831,7 +19832,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="165" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
         <v>264</v>
       </c>
@@ -19944,7 +19945,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="166" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
         <v>265</v>
       </c>
@@ -20057,7 +20058,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="167" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
         <v>266</v>
       </c>
@@ -20170,7 +20171,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="168" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
         <v>267</v>
       </c>
@@ -20275,7 +20276,7 @@
       <c r="AL168" s="2"/>
       <c r="AM168" s="2"/>
     </row>
-    <row r="169" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
         <v>268</v>
       </c>
@@ -20380,7 +20381,7 @@
       <c r="AL169" s="2"/>
       <c r="AM169" s="2"/>
     </row>
-    <row r="170" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
         <v>269</v>
       </c>
@@ -20485,7 +20486,7 @@
       <c r="AL170" s="2"/>
       <c r="AM170" s="2"/>
     </row>
-    <row r="171" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>270</v>
       </c>
@@ -20590,7 +20591,7 @@
       <c r="AL171" s="2"/>
       <c r="AM171" s="2"/>
     </row>
-    <row r="172" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
         <v>271</v>
       </c>
@@ -20695,7 +20696,7 @@
       <c r="AL172" s="2"/>
       <c r="AM172" s="2"/>
     </row>
-    <row r="173" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
         <v>272</v>
       </c>
@@ -20746,7 +20747,7 @@
       <c r="AF173" s="2"/>
       <c r="AG173" s="2"/>
     </row>
-    <row r="174" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
         <v>273</v>
       </c>
@@ -20797,7 +20798,7 @@
       <c r="AF174" s="2"/>
       <c r="AG174" s="2"/>
     </row>
-    <row r="175" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
         <v>274</v>
       </c>
@@ -20848,7 +20849,7 @@
       <c r="AF175" s="2"/>
       <c r="AG175" s="2"/>
     </row>
-    <row r="176" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>275</v>
       </c>
@@ -20899,7 +20900,7 @@
       <c r="AF176" s="2"/>
       <c r="AG176" s="2"/>
     </row>
-    <row r="177" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
         <v>276</v>
       </c>
@@ -21017,7 +21018,7 @@
       </c>
       <c r="AN177" s="47"/>
     </row>
-    <row r="178" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
         <v>277</v>
       </c>
@@ -21135,7 +21136,7 @@
       </c>
       <c r="AN178" s="47"/>
     </row>
-    <row r="179" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>278</v>
       </c>
@@ -21253,7 +21254,7 @@
       </c>
       <c r="AN179" s="47"/>
     </row>
-    <row r="180" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
         <v>279</v>
       </c>
@@ -21371,7 +21372,7 @@
       </c>
       <c r="AN180" s="47"/>
     </row>
-    <row r="181" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
         <v>280</v>
       </c>
@@ -21489,7 +21490,7 @@
       </c>
       <c r="AN181" s="47"/>
     </row>
-    <row r="182" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
         <v>281</v>
       </c>
@@ -21607,7 +21608,7 @@
       </c>
       <c r="AN182" s="47"/>
     </row>
-    <row r="183" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
         <v>282</v>
       </c>
@@ -21725,7 +21726,7 @@
       </c>
       <c r="AN183" s="47"/>
     </row>
-    <row r="184" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
         <v>283</v>
       </c>
@@ -21843,7 +21844,7 @@
       </c>
       <c r="AN184" s="47"/>
     </row>
-    <row r="185" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
         <v>284</v>
       </c>
@@ -21961,7 +21962,7 @@
       </c>
       <c r="AN185" s="47"/>
     </row>
-    <row r="186" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
         <v>285</v>
       </c>
@@ -22074,7 +22075,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="6" t="s">
         <v>286</v>
       </c>
@@ -22187,7 +22188,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
         <v>287</v>
       </c>
@@ -22300,7 +22301,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="6" t="s">
         <v>288</v>
       </c>
@@ -22413,7 +22414,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
         <v>289</v>
       </c>
@@ -22518,7 +22519,7 @@
       <c r="AL190" s="2"/>
       <c r="AM190" s="2"/>
     </row>
-    <row r="191" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
         <v>290</v>
       </c>
@@ -22623,7 +22624,7 @@
       <c r="AL191" s="2"/>
       <c r="AM191" s="2"/>
     </row>
-    <row r="192" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
         <v>291</v>
       </c>
@@ -22728,7 +22729,7 @@
       <c r="AL192" s="2"/>
       <c r="AM192" s="2"/>
     </row>
-    <row r="193" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
         <v>292</v>
       </c>
@@ -22833,7 +22834,7 @@
       <c r="AL193" s="2"/>
       <c r="AM193" s="2"/>
     </row>
-    <row r="194" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
         <v>295</v>
       </c>
@@ -22938,7 +22939,7 @@
       <c r="AL194" s="2"/>
       <c r="AM194" s="2"/>
     </row>
-    <row r="195" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="8" t="s">
         <v>293</v>
       </c>
@@ -23043,7 +23044,7 @@
       <c r="AL195" s="2"/>
       <c r="AM195" s="2"/>
     </row>
-    <row r="196" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="8" t="s">
         <v>294</v>
       </c>
@@ -24692,8 +24693,8 @@
       <c r="H210" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I210" s="10" t="s">
-        <v>436</v>
+      <c r="I210" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="J210" s="18">
         <v>4.2</v>
@@ -24809,8 +24810,8 @@
       <c r="H211" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I211" s="10" t="s">
-        <v>436</v>
+      <c r="I211" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="J211" s="18">
         <v>4.2</v>
@@ -24926,8 +24927,8 @@
       <c r="H212" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I212" s="10" t="s">
-        <v>436</v>
+      <c r="I212" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="J212" s="18">
         <v>4.2</v>
@@ -25043,8 +25044,8 @@
       <c r="H213" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I213" s="10" t="s">
-        <v>436</v>
+      <c r="I213" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="J213" s="18">
         <v>4.2</v>
@@ -25160,8 +25161,8 @@
       <c r="H214" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I214" s="10" t="s">
-        <v>436</v>
+      <c r="I214" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="J214" s="18">
         <v>4.2</v>
@@ -25277,8 +25278,8 @@
       <c r="H215" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I215" s="10" t="s">
-        <v>436</v>
+      <c r="I215" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="J215" s="18">
         <v>4.2</v>
@@ -25628,8 +25629,8 @@
       <c r="H218" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I218" s="10" t="s">
-        <v>436</v>
+      <c r="I218" s="4" t="s">
+        <v>438</v>
       </c>
       <c r="J218" s="18">
         <v>6.5</v>
@@ -25741,8 +25742,8 @@
       <c r="H219" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I219" s="10" t="s">
-        <v>436</v>
+      <c r="I219" s="4" t="s">
+        <v>438</v>
       </c>
       <c r="J219" s="18">
         <v>6.5</v>
@@ -25855,7 +25856,7 @@
         <v>435</v>
       </c>
       <c r="I220" s="10" t="s">
-        <v>436</v>
+        <v>186</v>
       </c>
       <c r="J220" s="18">
         <v>2.8</v>
@@ -25968,7 +25969,7 @@
         <v>435</v>
       </c>
       <c r="I221" s="10" t="s">
-        <v>436</v>
+        <v>186</v>
       </c>
       <c r="J221" s="18">
         <v>2.8</v>
@@ -26081,7 +26082,7 @@
         <v>435</v>
       </c>
       <c r="I222" s="10" t="s">
-        <v>436</v>
+        <v>186</v>
       </c>
       <c r="J222" s="22">
         <v>6</v>
@@ -26198,7 +26199,7 @@
         <v>435</v>
       </c>
       <c r="I223" s="10" t="s">
-        <v>436</v>
+        <v>186</v>
       </c>
       <c r="J223" s="22">
         <v>6</v>
@@ -26315,7 +26316,7 @@
         <v>435</v>
       </c>
       <c r="I224" s="10" t="s">
-        <v>436</v>
+        <v>186</v>
       </c>
       <c r="J224" s="22">
         <v>6</v>
@@ -26432,7 +26433,7 @@
         <v>435</v>
       </c>
       <c r="I225" s="10" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="J225" s="22">
         <v>6</v>
@@ -26782,8 +26783,8 @@
       <c r="H228" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I228" s="10" t="s">
-        <v>436</v>
+      <c r="I228" s="4" t="s">
+        <v>438</v>
       </c>
       <c r="J228" s="22">
         <v>6.2</v>
@@ -26895,8 +26896,8 @@
       <c r="H229" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I229" s="10" t="s">
-        <v>436</v>
+      <c r="I229" s="4" t="s">
+        <v>438</v>
       </c>
       <c r="J229" s="22">
         <v>6.2</v>
@@ -27009,7 +27010,7 @@
         <v>435</v>
       </c>
       <c r="I230" s="10" t="s">
-        <v>436</v>
+        <v>186</v>
       </c>
       <c r="J230" s="22">
         <v>2.7</v>
@@ -27122,7 +27123,7 @@
         <v>435</v>
       </c>
       <c r="I231" s="10" t="s">
-        <v>436</v>
+        <v>186</v>
       </c>
       <c r="J231" s="22">
         <v>2.7</v>
@@ -42530,6 +42531,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="F1:F373" xr:uid="{F1236420-0C1C-4AE2-B76E-36106E5A71DC}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="S"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -45677,8 +45685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA7E222-8FD4-4195-BBDF-94274DD187A7}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add files with 95% threshold, changed script to analyze 95% data, corrected mistake in met file
</commit_message>
<xml_diff>
--- a/data/met.xlsx
+++ b/data/met.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspkaur\Google Drive\Metagenomics\pico_comb_run\pico\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator/Documents/jaspreet/pico/pico_comb_run/pico/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42072BBE-276A-4EC9-A53B-DD03A5C114A5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32460" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="with_just_pg_envt" sheetId="13" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">envt_comp!$C$1:$C$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$A$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">with_just_pg_envt!$F$1:$F$373</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">with_just_pg_envt!$B$1:$C$373</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1920,25 +1919,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AN373"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="12" ySplit="20" topLeftCell="M350" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="20" topLeftCell="M358" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="K369" sqref="K369"/>
+      <selection pane="bottomRight" activeCell="I230" sqref="I230:I231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="9" width="11.140625" style="54" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" style="54" customWidth="1"/>
+    <col min="10" max="10" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2057,7 +2055,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2174,7 +2172,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="3" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>422</v>
       </c>
@@ -2227,7 +2225,7 @@
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
     </row>
-    <row r="4" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2344,7 +2342,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="5" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2461,7 +2459,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="6" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2578,7 +2576,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="7" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2695,7 +2693,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="8" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2812,7 +2810,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="9" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2929,7 +2927,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="10" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -3046,7 +3044,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="11" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -3163,7 +3161,7 @@
         <v>0.106641366223909</v>
       </c>
     </row>
-    <row r="12" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -3280,7 +3278,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -3397,7 +3395,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -3514,7 +3512,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -3631,7 +3629,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3748,7 +3746,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3865,7 +3863,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -3982,7 +3980,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -4099,7 +4097,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -4216,7 +4214,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -4333,7 +4331,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -4450,7 +4448,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -4567,7 +4565,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -4684,7 +4682,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -4801,7 +4799,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -4918,7 +4916,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -5035,7 +5033,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -5152,7 +5150,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -5265,7 +5263,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="30" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -5378,7 +5376,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="31" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -5491,7 +5489,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="32" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -5604,7 +5602,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="33" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -5717,7 +5715,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="34" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -5830,7 +5828,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="35" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -5943,7 +5941,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="36" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -6056,7 +6054,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="37" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -6169,7 +6167,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="38" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -6282,7 +6280,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="39" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -6395,7 +6393,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="40" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -6508,7 +6506,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="41" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
@@ -6625,7 +6623,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="42" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -6742,7 +6740,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="43" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
@@ -6859,7 +6857,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="44" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -6976,7 +6974,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="45" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
@@ -7089,7 +7087,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="46" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
@@ -7202,7 +7200,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="47" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -7315,7 +7313,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="48" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -7428,7 +7426,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="49" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -7545,7 +7543,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="50" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -7662,7 +7660,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="51" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -7779,7 +7777,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="52" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -7896,7 +7894,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="53" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -8013,7 +8011,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="54" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
@@ -8130,7 +8128,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="55" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
@@ -8247,7 +8245,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="56" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
@@ -8364,7 +8362,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="57" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>61</v>
       </c>
@@ -8481,7 +8479,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="58" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>62</v>
       </c>
@@ -8598,7 +8596,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="59" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
@@ -8715,7 +8713,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="60" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
@@ -8828,7 +8826,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="61" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>65</v>
       </c>
@@ -8941,7 +8939,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="62" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
@@ -9054,7 +9052,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="63" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
@@ -9167,7 +9165,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="64" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>68</v>
       </c>
@@ -9280,7 +9278,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="65" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>69</v>
       </c>
@@ -9393,7 +9391,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="66" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
@@ -9506,7 +9504,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="67" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
@@ -9619,7 +9617,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="68" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
@@ -9732,7 +9730,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="69" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
@@ -9845,7 +9843,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="70" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>423</v>
       </c>
@@ -9898,7 +9896,7 @@
       <c r="AL70" s="2"/>
       <c r="AM70" s="2"/>
     </row>
-    <row r="71" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>181</v>
       </c>
@@ -10003,7 +10001,7 @@
       <c r="AL71" s="3"/>
       <c r="AM71" s="3"/>
     </row>
-    <row r="72" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>182</v>
       </c>
@@ -10108,7 +10106,7 @@
       <c r="AL72" s="3"/>
       <c r="AM72" s="3"/>
     </row>
-    <row r="73" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>183</v>
       </c>
@@ -10213,7 +10211,7 @@
       <c r="AL73" s="3"/>
       <c r="AM73" s="3"/>
     </row>
-    <row r="74" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>74</v>
       </c>
@@ -10318,7 +10316,7 @@
       <c r="AL74" s="3"/>
       <c r="AM74" s="3"/>
     </row>
-    <row r="75" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>75</v>
       </c>
@@ -10423,7 +10421,7 @@
       <c r="AL75" s="2"/>
       <c r="AM75" s="2"/>
     </row>
-    <row r="76" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>76</v>
       </c>
@@ -10528,7 +10526,7 @@
       <c r="AL76" s="2"/>
       <c r="AM76" s="2"/>
     </row>
-    <row r="77" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>77</v>
       </c>
@@ -10633,7 +10631,7 @@
       <c r="AL77" s="2"/>
       <c r="AM77" s="2"/>
     </row>
-    <row r="78" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -10684,7 +10682,7 @@
       <c r="AF78" s="2"/>
       <c r="AG78" s="2"/>
     </row>
-    <row r="79" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>79</v>
       </c>
@@ -10735,7 +10733,7 @@
       <c r="AF79" s="2"/>
       <c r="AG79" s="2"/>
     </row>
-    <row r="80" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>80</v>
       </c>
@@ -10786,7 +10784,7 @@
       <c r="AF80" s="2"/>
       <c r="AG80" s="2"/>
     </row>
-    <row r="81" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>81</v>
       </c>
@@ -10837,7 +10835,7 @@
       <c r="AF81" s="2"/>
       <c r="AG81" s="2"/>
     </row>
-    <row r="82" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>82</v>
       </c>
@@ -10888,7 +10886,7 @@
       <c r="AF82" s="2"/>
       <c r="AG82" s="2"/>
     </row>
-    <row r="83" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>83</v>
       </c>
@@ -10939,7 +10937,7 @@
       <c r="AF83" s="2"/>
       <c r="AG83" s="2"/>
     </row>
-    <row r="84" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>84</v>
       </c>
@@ -10990,7 +10988,7 @@
       <c r="AF84" s="2"/>
       <c r="AG84" s="2"/>
     </row>
-    <row r="85" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>85</v>
       </c>
@@ -11041,7 +11039,7 @@
       <c r="AF85" s="2"/>
       <c r="AG85" s="2"/>
     </row>
-    <row r="86" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>86</v>
       </c>
@@ -11092,7 +11090,7 @@
       <c r="AF86" s="2"/>
       <c r="AG86" s="2"/>
     </row>
-    <row r="87" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>87</v>
       </c>
@@ -11143,7 +11141,7 @@
       <c r="AF87" s="2"/>
       <c r="AG87" s="2"/>
     </row>
-    <row r="88" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>88</v>
       </c>
@@ -11194,7 +11192,7 @@
       <c r="AF88" s="2"/>
       <c r="AG88" s="2"/>
     </row>
-    <row r="89" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>89</v>
       </c>
@@ -11245,7 +11243,7 @@
       <c r="AF89" s="2"/>
       <c r="AG89" s="2"/>
     </row>
-    <row r="90" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -11362,7 +11360,7 @@
         <v>6.1917808219178097E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>91</v>
       </c>
@@ -11475,7 +11473,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>92</v>
       </c>
@@ -11588,7 +11586,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>93</v>
       </c>
@@ -11701,7 +11699,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>94</v>
       </c>
@@ -11806,7 +11804,7 @@
       <c r="AL94" s="2"/>
       <c r="AM94" s="2"/>
     </row>
-    <row r="95" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -11911,7 +11909,7 @@
       <c r="AL95" s="2"/>
       <c r="AM95" s="2"/>
     </row>
-    <row r="96" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>96</v>
       </c>
@@ -12016,7 +12014,7 @@
       <c r="AL96" s="2"/>
       <c r="AM96" s="2"/>
     </row>
-    <row r="97" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>97</v>
       </c>
@@ -12121,7 +12119,7 @@
       <c r="AL97" s="2"/>
       <c r="AM97" s="2"/>
     </row>
-    <row r="98" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>98</v>
       </c>
@@ -12226,7 +12224,7 @@
       <c r="AL98" s="2"/>
       <c r="AM98" s="2"/>
     </row>
-    <row r="99" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>99</v>
       </c>
@@ -12331,7 +12329,7 @@
       <c r="AL99" s="2"/>
       <c r="AM99" s="2"/>
     </row>
-    <row r="100" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>199</v>
       </c>
@@ -12448,7 +12446,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="101" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>200</v>
       </c>
@@ -12565,7 +12563,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="102" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>201</v>
       </c>
@@ -12682,7 +12680,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="103" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>202</v>
       </c>
@@ -12799,7 +12797,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="104" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>203</v>
       </c>
@@ -12916,7 +12914,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="105" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>204</v>
       </c>
@@ -13033,7 +13031,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="106" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>205</v>
       </c>
@@ -13150,7 +13148,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="107" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>206</v>
       </c>
@@ -13267,7 +13265,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="108" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>207</v>
       </c>
@@ -13384,7 +13382,7 @@
         <v>0.106641366223909</v>
       </c>
     </row>
-    <row r="109" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>208</v>
       </c>
@@ -13501,7 +13499,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
         <v>209</v>
       </c>
@@ -13618,7 +13616,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
         <v>210</v>
       </c>
@@ -13735,7 +13733,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
         <v>211</v>
       </c>
@@ -13852,7 +13850,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
         <v>212</v>
       </c>
@@ -13969,7 +13967,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
         <v>213</v>
       </c>
@@ -14086,7 +14084,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
         <v>214</v>
       </c>
@@ -14203,7 +14201,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
         <v>215</v>
       </c>
@@ -14320,7 +14318,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
         <v>216</v>
       </c>
@@ -14437,7 +14435,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
         <v>217</v>
       </c>
@@ -14554,7 +14552,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
         <v>218</v>
       </c>
@@ -14671,7 +14669,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
         <v>219</v>
       </c>
@@ -14788,7 +14786,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
         <v>220</v>
       </c>
@@ -14905,7 +14903,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
         <v>221</v>
       </c>
@@ -15022,7 +15020,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
         <v>222</v>
       </c>
@@ -15139,7 +15137,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A124" s="6" t="s">
         <v>223</v>
       </c>
@@ -15256,7 +15254,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
         <v>224</v>
       </c>
@@ -15373,7 +15371,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
         <v>225</v>
       </c>
@@ -15490,7 +15488,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
         <v>226</v>
       </c>
@@ -15603,7 +15601,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="128" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
         <v>227</v>
       </c>
@@ -15716,7 +15714,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="129" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A129" s="6" t="s">
         <v>228</v>
       </c>
@@ -15829,7 +15827,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="130" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
         <v>229</v>
       </c>
@@ -15942,7 +15940,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="131" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
         <v>230</v>
       </c>
@@ -16055,7 +16053,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="132" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
         <v>231</v>
       </c>
@@ -16168,7 +16166,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="133" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
         <v>232</v>
       </c>
@@ -16281,7 +16279,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="134" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A134" s="6" t="s">
         <v>233</v>
       </c>
@@ -16394,7 +16392,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="135" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A135" s="6" t="s">
         <v>234</v>
       </c>
@@ -16507,7 +16505,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="136" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
         <v>235</v>
       </c>
@@ -16620,7 +16618,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="137" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
         <v>236</v>
       </c>
@@ -16733,7 +16731,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="138" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
         <v>237</v>
       </c>
@@ -16846,7 +16844,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="139" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A139" s="6" t="s">
         <v>238</v>
       </c>
@@ -16959,7 +16957,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="140" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
         <v>239</v>
       </c>
@@ -17076,7 +17074,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="141" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
         <v>240</v>
       </c>
@@ -17193,7 +17191,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="142" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
         <v>241</v>
       </c>
@@ -17310,7 +17308,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="143" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
         <v>242</v>
       </c>
@@ -17427,7 +17425,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="144" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
         <v>243</v>
       </c>
@@ -17540,7 +17538,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="145" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
         <v>244</v>
       </c>
@@ -17653,7 +17651,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="146" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
         <v>245</v>
       </c>
@@ -17766,7 +17764,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="147" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
         <v>246</v>
       </c>
@@ -17871,7 +17869,7 @@
       <c r="AL147" s="2"/>
       <c r="AM147" s="2"/>
     </row>
-    <row r="148" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
         <v>247</v>
       </c>
@@ -17988,7 +17986,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="149" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A149" s="6" t="s">
         <v>248</v>
       </c>
@@ -18105,7 +18103,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="150" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A150" s="6" t="s">
         <v>249</v>
       </c>
@@ -18222,7 +18220,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="151" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
         <v>250</v>
       </c>
@@ -18339,7 +18337,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="152" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A152" s="6" t="s">
         <v>251</v>
       </c>
@@ -18456,7 +18454,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="153" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
         <v>252</v>
       </c>
@@ -18573,7 +18571,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="154" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A154" s="6" t="s">
         <v>253</v>
       </c>
@@ -18690,7 +18688,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="155" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
         <v>254</v>
       </c>
@@ -18807,7 +18805,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="156" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
         <v>255</v>
       </c>
@@ -18924,7 +18922,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="157" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
         <v>256</v>
       </c>
@@ -19041,7 +19039,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="158" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
         <v>257</v>
       </c>
@@ -19154,7 +19152,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="159" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A159" s="6" t="s">
         <v>258</v>
       </c>
@@ -19267,7 +19265,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="160" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
         <v>259</v>
       </c>
@@ -19380,7 +19378,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="161" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A161" s="6" t="s">
         <v>260</v>
       </c>
@@ -19493,7 +19491,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="162" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A162" s="6" t="s">
         <v>261</v>
       </c>
@@ -19606,7 +19604,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="163" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A163" s="6" t="s">
         <v>262</v>
       </c>
@@ -19719,7 +19717,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="164" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A164" s="6" t="s">
         <v>263</v>
       </c>
@@ -19832,7 +19830,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="165" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A165" s="6" t="s">
         <v>264</v>
       </c>
@@ -19945,7 +19943,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="166" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A166" s="6" t="s">
         <v>265</v>
       </c>
@@ -20058,7 +20056,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="167" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
         <v>266</v>
       </c>
@@ -20171,7 +20169,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="168" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A168" s="6" t="s">
         <v>267</v>
       </c>
@@ -20276,7 +20274,7 @@
       <c r="AL168" s="2"/>
       <c r="AM168" s="2"/>
     </row>
-    <row r="169" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A169" s="6" t="s">
         <v>268</v>
       </c>
@@ -20381,7 +20379,7 @@
       <c r="AL169" s="2"/>
       <c r="AM169" s="2"/>
     </row>
-    <row r="170" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A170" s="6" t="s">
         <v>269</v>
       </c>
@@ -20486,7 +20484,7 @@
       <c r="AL170" s="2"/>
       <c r="AM170" s="2"/>
     </row>
-    <row r="171" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A171" s="6" t="s">
         <v>270</v>
       </c>
@@ -20591,7 +20589,7 @@
       <c r="AL171" s="2"/>
       <c r="AM171" s="2"/>
     </row>
-    <row r="172" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
         <v>271</v>
       </c>
@@ -20696,7 +20694,7 @@
       <c r="AL172" s="2"/>
       <c r="AM172" s="2"/>
     </row>
-    <row r="173" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
         <v>272</v>
       </c>
@@ -20747,7 +20745,7 @@
       <c r="AF173" s="2"/>
       <c r="AG173" s="2"/>
     </row>
-    <row r="174" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A174" s="6" t="s">
         <v>273</v>
       </c>
@@ -20798,7 +20796,7 @@
       <c r="AF174" s="2"/>
       <c r="AG174" s="2"/>
     </row>
-    <row r="175" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A175" s="6" t="s">
         <v>274</v>
       </c>
@@ -20849,7 +20847,7 @@
       <c r="AF175" s="2"/>
       <c r="AG175" s="2"/>
     </row>
-    <row r="176" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A176" s="6" t="s">
         <v>275</v>
       </c>
@@ -20900,7 +20898,7 @@
       <c r="AF176" s="2"/>
       <c r="AG176" s="2"/>
     </row>
-    <row r="177" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A177" s="6" t="s">
         <v>276</v>
       </c>
@@ -21018,7 +21016,7 @@
       </c>
       <c r="AN177" s="47"/>
     </row>
-    <row r="178" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A178" s="6" t="s">
         <v>277</v>
       </c>
@@ -21136,7 +21134,7 @@
       </c>
       <c r="AN178" s="47"/>
     </row>
-    <row r="179" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A179" s="6" t="s">
         <v>278</v>
       </c>
@@ -21254,7 +21252,7 @@
       </c>
       <c r="AN179" s="47"/>
     </row>
-    <row r="180" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A180" s="6" t="s">
         <v>279</v>
       </c>
@@ -21372,7 +21370,7 @@
       </c>
       <c r="AN180" s="47"/>
     </row>
-    <row r="181" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A181" s="6" t="s">
         <v>280</v>
       </c>
@@ -21490,7 +21488,7 @@
       </c>
       <c r="AN181" s="47"/>
     </row>
-    <row r="182" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A182" s="6" t="s">
         <v>281</v>
       </c>
@@ -21608,7 +21606,7 @@
       </c>
       <c r="AN182" s="47"/>
     </row>
-    <row r="183" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A183" s="6" t="s">
         <v>282</v>
       </c>
@@ -21726,7 +21724,7 @@
       </c>
       <c r="AN183" s="47"/>
     </row>
-    <row r="184" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A184" s="6" t="s">
         <v>283</v>
       </c>
@@ -21844,7 +21842,7 @@
       </c>
       <c r="AN184" s="47"/>
     </row>
-    <row r="185" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A185" s="6" t="s">
         <v>284</v>
       </c>
@@ -21962,7 +21960,7 @@
       </c>
       <c r="AN185" s="47"/>
     </row>
-    <row r="186" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A186" s="6" t="s">
         <v>285</v>
       </c>
@@ -22075,7 +22073,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A187" s="6" t="s">
         <v>286</v>
       </c>
@@ -22188,7 +22186,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A188" s="6" t="s">
         <v>287</v>
       </c>
@@ -22301,7 +22299,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A189" s="6" t="s">
         <v>288</v>
       </c>
@@ -22414,7 +22412,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A190" s="6" t="s">
         <v>289</v>
       </c>
@@ -22519,7 +22517,7 @@
       <c r="AL190" s="2"/>
       <c r="AM190" s="2"/>
     </row>
-    <row r="191" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A191" s="6" t="s">
         <v>290</v>
       </c>
@@ -22624,7 +22622,7 @@
       <c r="AL191" s="2"/>
       <c r="AM191" s="2"/>
     </row>
-    <row r="192" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A192" s="6" t="s">
         <v>291</v>
       </c>
@@ -22729,7 +22727,7 @@
       <c r="AL192" s="2"/>
       <c r="AM192" s="2"/>
     </row>
-    <row r="193" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A193" s="8" t="s">
         <v>292</v>
       </c>
@@ -22834,7 +22832,7 @@
       <c r="AL193" s="2"/>
       <c r="AM193" s="2"/>
     </row>
-    <row r="194" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A194" s="8" t="s">
         <v>295</v>
       </c>
@@ -22939,7 +22937,7 @@
       <c r="AL194" s="2"/>
       <c r="AM194" s="2"/>
     </row>
-    <row r="195" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A195" s="8" t="s">
         <v>293</v>
       </c>
@@ -23044,7 +23042,7 @@
       <c r="AL195" s="2"/>
       <c r="AM195" s="2"/>
     </row>
-    <row r="196" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A196" s="8" t="s">
         <v>294</v>
       </c>
@@ -23149,7 +23147,7 @@
       <c r="AL196" s="2"/>
       <c r="AM196" s="2"/>
     </row>
-    <row r="197" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>100</v>
       </c>
@@ -23266,7 +23264,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="198" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>101</v>
       </c>
@@ -23383,7 +23381,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="199" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>102</v>
       </c>
@@ -23500,7 +23498,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="200" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>103</v>
       </c>
@@ -23617,7 +23615,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="201" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>104</v>
       </c>
@@ -23734,7 +23732,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="202" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>105</v>
       </c>
@@ -23851,7 +23849,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="203" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>106</v>
       </c>
@@ -23968,7 +23966,7 @@
         <v>0.106641366223909</v>
       </c>
     </row>
-    <row r="204" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>107</v>
       </c>
@@ -24085,7 +24083,7 @@
         <v>0.106641366223909</v>
       </c>
     </row>
-    <row r="205" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>108</v>
       </c>
@@ -24202,7 +24200,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>109</v>
       </c>
@@ -24319,7 +24317,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>110</v>
       </c>
@@ -24436,7 +24434,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>111</v>
       </c>
@@ -24553,7 +24551,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>112</v>
       </c>
@@ -24670,7 +24668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
         <v>113</v>
       </c>
@@ -24693,7 +24691,7 @@
       <c r="H210" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I210" s="4" t="s">
+      <c r="I210" s="10" t="s">
         <v>186</v>
       </c>
       <c r="J210" s="18">
@@ -24787,7 +24785,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>114</v>
       </c>
@@ -24810,7 +24808,7 @@
       <c r="H211" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I211" s="4" t="s">
+      <c r="I211" s="10" t="s">
         <v>186</v>
       </c>
       <c r="J211" s="18">
@@ -24904,7 +24902,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>115</v>
       </c>
@@ -24927,7 +24925,7 @@
       <c r="H212" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I212" s="4" t="s">
+      <c r="I212" s="10" t="s">
         <v>186</v>
       </c>
       <c r="J212" s="18">
@@ -25021,7 +25019,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>116</v>
       </c>
@@ -25044,7 +25042,7 @@
       <c r="H213" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I213" s="4" t="s">
+      <c r="I213" s="10" t="s">
         <v>186</v>
       </c>
       <c r="J213" s="18">
@@ -25138,7 +25136,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
         <v>117</v>
       </c>
@@ -25161,7 +25159,7 @@
       <c r="H214" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I214" s="4" t="s">
+      <c r="I214" s="10" t="s">
         <v>186</v>
       </c>
       <c r="J214" s="18">
@@ -25255,7 +25253,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>118</v>
       </c>
@@ -25278,7 +25276,7 @@
       <c r="H215" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I215" s="4" t="s">
+      <c r="I215" s="10" t="s">
         <v>186</v>
       </c>
       <c r="J215" s="18">
@@ -25372,7 +25370,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
         <v>119</v>
       </c>
@@ -25489,7 +25487,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>120</v>
       </c>
@@ -25606,7 +25604,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
         <v>121</v>
       </c>
@@ -25719,7 +25717,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="219" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>122</v>
       </c>
@@ -25832,7 +25830,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="220" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
         <v>123</v>
       </c>
@@ -25945,7 +25943,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="221" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>124</v>
       </c>
@@ -26058,7 +26056,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="222" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>125</v>
       </c>
@@ -26175,7 +26173,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="223" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>126</v>
       </c>
@@ -26292,7 +26290,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="224" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>127</v>
       </c>
@@ -26409,7 +26407,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="225" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>128</v>
       </c>
@@ -26433,7 +26431,7 @@
         <v>435</v>
       </c>
       <c r="I225" s="10" t="s">
-        <v>438</v>
+        <v>186</v>
       </c>
       <c r="J225" s="22">
         <v>6</v>
@@ -26526,7 +26524,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="226" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>129</v>
       </c>
@@ -26643,7 +26641,7 @@
         <v>0.127671232876712</v>
       </c>
     </row>
-    <row r="227" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>130</v>
       </c>
@@ -26760,7 +26758,7 @@
         <v>0.127671232876712</v>
       </c>
     </row>
-    <row r="228" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
         <v>131</v>
       </c>
@@ -26873,7 +26871,7 @@
         <v>0.104781420765027</v>
       </c>
     </row>
-    <row r="229" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>132</v>
       </c>
@@ -26986,7 +26984,7 @@
         <v>0.104781420765027</v>
       </c>
     </row>
-    <row r="230" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>133</v>
       </c>
@@ -27099,7 +27097,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="231" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>134</v>
       </c>
@@ -27212,7 +27210,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="232" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>135</v>
       </c>
@@ -27317,7 +27315,7 @@
       <c r="AL232" s="2"/>
       <c r="AM232" s="2"/>
     </row>
-    <row r="233" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>136</v>
       </c>
@@ -27422,7 +27420,7 @@
       <c r="AL233" s="2"/>
       <c r="AM233" s="2"/>
     </row>
-    <row r="234" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
         <v>137</v>
       </c>
@@ -27527,7 +27525,7 @@
       <c r="AL234" s="2"/>
       <c r="AM234" s="2"/>
     </row>
-    <row r="235" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>138</v>
       </c>
@@ -27632,7 +27630,7 @@
       <c r="AL235" s="2"/>
       <c r="AM235" s="2"/>
     </row>
-    <row r="236" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A236" s="28" t="s">
         <v>139</v>
       </c>
@@ -27731,7 +27729,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="237" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A237" s="28" t="s">
         <v>140</v>
       </c>
@@ -27830,7 +27828,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="238" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A238" s="28" t="s">
         <v>141</v>
       </c>
@@ -27929,7 +27927,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="239" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A239" s="28" t="s">
         <v>142</v>
       </c>
@@ -28028,7 +28026,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="240" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A240" s="28" t="s">
         <v>143</v>
       </c>
@@ -28127,7 +28125,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="241" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A241" s="28" t="s">
         <v>144</v>
       </c>
@@ -28226,7 +28224,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="242" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>145</v>
       </c>
@@ -28343,7 +28341,7 @@
         <v>9.9022801302931604E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>146</v>
       </c>
@@ -28460,7 +28458,7 @@
         <v>9.9022801302931604E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
         <v>147</v>
       </c>
@@ -28577,7 +28575,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="245" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>148</v>
       </c>
@@ -28694,7 +28692,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="246" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>149</v>
       </c>
@@ -28811,7 +28809,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="247" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>150</v>
       </c>
@@ -28928,7 +28926,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="248" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>151</v>
       </c>
@@ -29045,7 +29043,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="249" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>152</v>
       </c>
@@ -29162,7 +29160,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="250" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>153</v>
       </c>
@@ -29275,7 +29273,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="251" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>154</v>
       </c>
@@ -29388,7 +29386,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="252" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>155</v>
       </c>
@@ -29501,7 +29499,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="253" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>156</v>
       </c>
@@ -29614,7 +29612,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="254" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>157</v>
       </c>
@@ -29719,7 +29717,7 @@
       <c r="AL254" s="2"/>
       <c r="AM254" s="2"/>
     </row>
-    <row r="255" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>158</v>
       </c>
@@ -29824,7 +29822,7 @@
       <c r="AL255" s="2"/>
       <c r="AM255" s="2"/>
     </row>
-    <row r="256" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>159</v>
       </c>
@@ -29929,7 +29927,7 @@
       <c r="AL256" s="2"/>
       <c r="AM256" s="2"/>
     </row>
-    <row r="257" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>160</v>
       </c>
@@ -30034,7 +30032,7 @@
       <c r="AL257" s="2"/>
       <c r="AM257" s="2"/>
     </row>
-    <row r="258" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>161</v>
       </c>
@@ -30139,7 +30137,7 @@
       <c r="AL258" s="2"/>
       <c r="AM258" s="2"/>
     </row>
-    <row r="259" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>162</v>
       </c>
@@ -30244,7 +30242,7 @@
       <c r="AL259" s="2"/>
       <c r="AM259" s="2"/>
     </row>
-    <row r="260" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>163</v>
       </c>
@@ -30349,7 +30347,7 @@
       <c r="AL260" s="2"/>
       <c r="AM260" s="2"/>
     </row>
-    <row r="261" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>164</v>
       </c>
@@ -30454,7 +30452,7 @@
       <c r="AL261" s="2"/>
       <c r="AM261" s="2"/>
     </row>
-    <row r="262" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>165</v>
       </c>
@@ -30572,7 +30570,7 @@
       </c>
       <c r="AN262" s="47"/>
     </row>
-    <row r="263" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>166</v>
       </c>
@@ -30690,7 +30688,7 @@
       </c>
       <c r="AN263" s="47"/>
     </row>
-    <row r="264" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>167</v>
       </c>
@@ -30808,7 +30806,7 @@
       </c>
       <c r="AN264" s="47"/>
     </row>
-    <row r="265" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>168</v>
       </c>
@@ -30926,7 +30924,7 @@
       </c>
       <c r="AN265" s="47"/>
     </row>
-    <row r="266" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>169</v>
       </c>
@@ -31043,7 +31041,7 @@
         <v>6.1917808219178097E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>170</v>
       </c>
@@ -31160,7 +31158,7 @@
         <v>6.1917808219178097E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>171</v>
       </c>
@@ -31273,7 +31271,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>172</v>
       </c>
@@ -31386,7 +31384,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>173</v>
       </c>
@@ -31491,7 +31489,7 @@
       <c r="AL270" s="2"/>
       <c r="AM270" s="2"/>
     </row>
-    <row r="271" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>174</v>
       </c>
@@ -31596,7 +31594,7 @@
       <c r="AL271" s="2"/>
       <c r="AM271" s="2"/>
     </row>
-    <row r="272" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>175</v>
       </c>
@@ -31701,7 +31699,7 @@
       <c r="AL272" s="2"/>
       <c r="AM272" s="2"/>
     </row>
-    <row r="273" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>176</v>
       </c>
@@ -31806,7 +31804,7 @@
       <c r="AL273" s="2"/>
       <c r="AM273" s="2"/>
     </row>
-    <row r="274" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>177</v>
       </c>
@@ -31911,7 +31909,7 @@
       <c r="AL274" s="2"/>
       <c r="AM274" s="2"/>
     </row>
-    <row r="275" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>178</v>
       </c>
@@ -32016,7 +32014,7 @@
       <c r="AL275" s="2"/>
       <c r="AM275" s="2"/>
     </row>
-    <row r="276" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
         <v>179</v>
       </c>
@@ -32133,7 +32131,7 @@
         <v>5.4794520547945197E-3</v>
       </c>
     </row>
-    <row r="277" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>180</v>
       </c>
@@ -32250,7 +32248,7 @@
         <v>5.4794520547945197E-3</v>
       </c>
     </row>
-    <row r="278" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A278" s="5" t="s">
         <v>424</v>
       </c>
@@ -32303,7 +32301,7 @@
       <c r="AL278" s="2"/>
       <c r="AM278" s="2"/>
     </row>
-    <row r="279" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A279" s="5" t="s">
         <v>425</v>
       </c>
@@ -32356,7 +32354,7 @@
       <c r="AL279" s="2"/>
       <c r="AM279" s="2"/>
     </row>
-    <row r="280" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
         <v>184</v>
       </c>
@@ -32473,7 +32471,7 @@
         <v>7.1232876712328794E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>185</v>
       </c>
@@ -32590,7 +32588,7 @@
         <v>7.1232876712328794E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A282" s="7" t="s">
         <v>296</v>
       </c>
@@ -32707,7 +32705,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="283" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A283" s="7" t="s">
         <v>297</v>
       </c>
@@ -32824,7 +32822,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="284" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A284" s="7" t="s">
         <v>298</v>
       </c>
@@ -32941,7 +32939,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="285" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A285" s="7" t="s">
         <v>299</v>
       </c>
@@ -33058,7 +33056,7 @@
         <v>0.10948766603415599</v>
       </c>
     </row>
-    <row r="286" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A286" s="7" t="s">
         <v>426</v>
       </c>
@@ -33175,7 +33173,7 @@
         <v>0.106641366223909</v>
       </c>
     </row>
-    <row r="287" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A287" s="7" t="s">
         <v>427</v>
       </c>
@@ -33292,7 +33290,7 @@
         <v>0.106641366223909</v>
       </c>
     </row>
-    <row r="288" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A288" s="7" t="s">
         <v>300</v>
       </c>
@@ -33409,7 +33407,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="289" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A289" s="7" t="s">
         <v>301</v>
       </c>
@@ -33526,7 +33524,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A290" s="7" t="s">
         <v>302</v>
       </c>
@@ -33643,7 +33641,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="291" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A291" s="7" t="s">
         <v>303</v>
       </c>
@@ -33760,7 +33758,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="292" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A292" s="7" t="s">
         <v>304</v>
       </c>
@@ -33877,7 +33875,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="293" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A293" s="7" t="s">
         <v>305</v>
       </c>
@@ -33994,7 +33992,7 @@
         <v>4.26183844011142E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A294" s="7" t="s">
         <v>306</v>
       </c>
@@ -34111,7 +34109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A295" s="7" t="s">
         <v>307</v>
       </c>
@@ -34228,7 +34226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A296" s="7" t="s">
         <v>308</v>
       </c>
@@ -34345,7 +34343,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="297" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A297" s="7" t="s">
         <v>309</v>
       </c>
@@ -34462,7 +34460,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="298" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A298" s="7" t="s">
         <v>310</v>
       </c>
@@ -34579,7 +34577,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="299" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A299" s="7" t="s">
         <v>311</v>
       </c>
@@ -34696,7 +34694,7 @@
         <v>2.4489796024804202E-2</v>
       </c>
     </row>
-    <row r="300" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A300" s="7" t="s">
         <v>312</v>
       </c>
@@ -34813,7 +34811,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="301" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A301" s="7" t="s">
         <v>313</v>
       </c>
@@ -34930,7 +34928,7 @@
         <v>3.6923076923076899E-2</v>
       </c>
     </row>
-    <row r="302" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A302" s="7" t="s">
         <v>314</v>
       </c>
@@ -35043,7 +35041,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="303" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A303" s="7" t="s">
         <v>315</v>
       </c>
@@ -35156,7 +35154,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="304" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A304" s="7" t="s">
         <v>316</v>
       </c>
@@ -35269,7 +35267,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="305" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A305" s="7" t="s">
         <v>317</v>
       </c>
@@ -35382,7 +35380,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="306" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A306" s="7" t="s">
         <v>318</v>
       </c>
@@ -35499,7 +35497,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="307" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A307" s="7" t="s">
         <v>319</v>
       </c>
@@ -35616,7 +35614,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="308" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A308" s="7" t="s">
         <v>320</v>
       </c>
@@ -35733,7 +35731,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="309" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A309" s="7" t="s">
         <v>321</v>
       </c>
@@ -35850,7 +35848,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="310" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A310" s="7" t="s">
         <v>322</v>
       </c>
@@ -35967,7 +35965,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="311" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A311" s="7" t="s">
         <v>323</v>
       </c>
@@ -36084,7 +36082,7 @@
         <v>0.121095889398496</v>
       </c>
     </row>
-    <row r="312" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A312" s="7" t="s">
         <v>324</v>
       </c>
@@ -36201,7 +36199,7 @@
         <v>0.127671232876712</v>
       </c>
     </row>
-    <row r="313" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A313" s="7" t="s">
         <v>325</v>
       </c>
@@ -36318,7 +36316,7 @@
         <v>0.127671232876712</v>
       </c>
     </row>
-    <row r="314" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A314" s="7" t="s">
         <v>326</v>
       </c>
@@ -36431,7 +36429,7 @@
         <v>0.104781420765027</v>
       </c>
     </row>
-    <row r="315" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A315" s="7" t="s">
         <v>327</v>
       </c>
@@ -36544,7 +36542,7 @@
         <v>0.104781420765027</v>
       </c>
     </row>
-    <row r="316" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A316" s="7" t="s">
         <v>328</v>
       </c>
@@ -36657,7 +36655,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="317" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A317" s="7" t="s">
         <v>329</v>
       </c>
@@ -36770,7 +36768,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="318" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A318" s="7" t="s">
         <v>330</v>
       </c>
@@ -36875,7 +36873,7 @@
       <c r="AL318" s="2"/>
       <c r="AM318" s="2"/>
     </row>
-    <row r="319" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A319" s="7" t="s">
         <v>331</v>
       </c>
@@ -36980,7 +36978,7 @@
       <c r="AL319" s="2"/>
       <c r="AM319" s="2"/>
     </row>
-    <row r="320" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A320" s="7" t="s">
         <v>332</v>
       </c>
@@ -37085,7 +37083,7 @@
       <c r="AL320" s="2"/>
       <c r="AM320" s="2"/>
     </row>
-    <row r="321" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A321" s="7" t="s">
         <v>333</v>
       </c>
@@ -37190,7 +37188,7 @@
       <c r="AL321" s="2"/>
       <c r="AM321" s="2"/>
     </row>
-    <row r="322" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A322" s="7" t="s">
         <v>334</v>
       </c>
@@ -37295,7 +37293,7 @@
       <c r="AL322" s="2"/>
       <c r="AM322" s="2"/>
     </row>
-    <row r="323" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A323" s="7" t="s">
         <v>335</v>
       </c>
@@ -37400,7 +37398,7 @@
       <c r="AL323" s="2"/>
       <c r="AM323" s="2"/>
     </row>
-    <row r="324" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A324" s="7" t="s">
         <v>336</v>
       </c>
@@ -37499,7 +37497,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="325" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A325" s="7" t="s">
         <v>337</v>
       </c>
@@ -37598,7 +37596,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="326" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A326" s="7" t="s">
         <v>338</v>
       </c>
@@ -37697,7 +37695,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="327" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A327" s="7" t="s">
         <v>339</v>
       </c>
@@ -37796,7 +37794,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="328" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A328" s="7" t="s">
         <v>340</v>
       </c>
@@ -37913,7 +37911,7 @@
         <v>9.9022801302931604E-2</v>
       </c>
     </row>
-    <row r="329" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A329" s="7" t="s">
         <v>341</v>
       </c>
@@ -38030,7 +38028,7 @@
         <v>9.9022801302931604E-2</v>
       </c>
     </row>
-    <row r="330" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A330" s="7" t="s">
         <v>342</v>
       </c>
@@ -38147,7 +38145,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="331" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A331" s="7" t="s">
         <v>343</v>
       </c>
@@ -38264,7 +38262,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="332" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A332" s="7" t="s">
         <v>344</v>
       </c>
@@ -38381,7 +38379,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="333" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A333" s="7" t="s">
         <v>345</v>
       </c>
@@ -38498,7 +38496,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="334" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A334" s="7" t="s">
         <v>346</v>
       </c>
@@ -38615,7 +38613,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="335" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A335" s="7" t="s">
         <v>347</v>
       </c>
@@ -38732,7 +38730,7 @@
         <v>0.71098265895953805</v>
       </c>
     </row>
-    <row r="336" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A336" s="7" t="s">
         <v>348</v>
       </c>
@@ -38849,7 +38847,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="337" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A337" s="7" t="s">
         <v>349</v>
       </c>
@@ -38966,7 +38964,7 @@
         <v>0.63862332695984703</v>
       </c>
     </row>
-    <row r="338" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A338" s="7" t="s">
         <v>350</v>
       </c>
@@ -39079,7 +39077,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="339" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A339" s="7" t="s">
         <v>351</v>
       </c>
@@ -39192,7 +39190,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="340" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A340" s="7" t="s">
         <v>352</v>
       </c>
@@ -39305,7 +39303,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="341" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A341" s="7" t="s">
         <v>353</v>
       </c>
@@ -39418,7 +39416,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="342" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A342" s="7" t="s">
         <v>354</v>
       </c>
@@ -39523,7 +39521,7 @@
       <c r="AL342" s="2"/>
       <c r="AM342" s="2"/>
     </row>
-    <row r="343" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A343" s="7" t="s">
         <v>355</v>
       </c>
@@ -39628,7 +39626,7 @@
       <c r="AL343" s="2"/>
       <c r="AM343" s="2"/>
     </row>
-    <row r="344" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A344" s="7" t="s">
         <v>356</v>
       </c>
@@ -39733,7 +39731,7 @@
       <c r="AL344" s="2"/>
       <c r="AM344" s="2"/>
     </row>
-    <row r="345" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A345" s="7" t="s">
         <v>357</v>
       </c>
@@ -39838,7 +39836,7 @@
       <c r="AL345" s="2"/>
       <c r="AM345" s="2"/>
     </row>
-    <row r="346" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A346" s="7" t="s">
         <v>358</v>
       </c>
@@ -39943,7 +39941,7 @@
       <c r="AL346" s="2"/>
       <c r="AM346" s="2"/>
     </row>
-    <row r="347" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A347" s="7" t="s">
         <v>359</v>
       </c>
@@ -40048,7 +40046,7 @@
       <c r="AL347" s="2"/>
       <c r="AM347" s="2"/>
     </row>
-    <row r="348" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A348" s="7" t="s">
         <v>360</v>
       </c>
@@ -40166,7 +40164,7 @@
       </c>
       <c r="AN348" s="47"/>
     </row>
-    <row r="349" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A349" s="7" t="s">
         <v>361</v>
       </c>
@@ -40284,7 +40282,7 @@
       </c>
       <c r="AN349" s="47"/>
     </row>
-    <row r="350" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A350" s="7" t="s">
         <v>362</v>
       </c>
@@ -40402,7 +40400,7 @@
       </c>
       <c r="AN350" s="47"/>
     </row>
-    <row r="351" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A351" s="7" t="s">
         <v>363</v>
       </c>
@@ -40520,7 +40518,7 @@
       </c>
       <c r="AN351" s="47"/>
     </row>
-    <row r="352" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A352" s="7" t="s">
         <v>364</v>
       </c>
@@ -40638,7 +40636,7 @@
       </c>
       <c r="AN352" s="47"/>
     </row>
-    <row r="353" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A353" s="7" t="s">
         <v>365</v>
       </c>
@@ -40756,7 +40754,7 @@
       </c>
       <c r="AN353" s="47"/>
     </row>
-    <row r="354" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A354" s="7" t="s">
         <v>366</v>
       </c>
@@ -40873,7 +40871,7 @@
         <v>6.1917808219178097E-2</v>
       </c>
     </row>
-    <row r="355" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A355" s="7" t="s">
         <v>367</v>
       </c>
@@ -40990,7 +40988,7 @@
         <v>6.1917808219178097E-2</v>
       </c>
     </row>
-    <row r="356" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A356" s="7" t="s">
         <v>368</v>
       </c>
@@ -41103,7 +41101,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="357" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A357" s="7" t="s">
         <v>369</v>
       </c>
@@ -41216,7 +41214,7 @@
         <v>2.4972677595628399E-2</v>
       </c>
     </row>
-    <row r="358" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A358" s="7" t="s">
         <v>370</v>
       </c>
@@ -41321,7 +41319,7 @@
       <c r="AL358" s="2"/>
       <c r="AM358" s="2"/>
     </row>
-    <row r="359" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A359" s="7" t="s">
         <v>371</v>
       </c>
@@ -41426,7 +41424,7 @@
       <c r="AL359" s="2"/>
       <c r="AM359" s="2"/>
     </row>
-    <row r="360" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A360" s="7" t="s">
         <v>372</v>
       </c>
@@ -41531,7 +41529,7 @@
       <c r="AL360" s="2"/>
       <c r="AM360" s="2"/>
     </row>
-    <row r="361" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A361" s="7" t="s">
         <v>373</v>
       </c>
@@ -41636,7 +41634,7 @@
       <c r="AL361" s="2"/>
       <c r="AM361" s="2"/>
     </row>
-    <row r="362" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A362" s="7" t="s">
         <v>374</v>
       </c>
@@ -41741,7 +41739,7 @@
       <c r="AL362" s="2"/>
       <c r="AM362" s="2"/>
     </row>
-    <row r="363" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A363" s="7" t="s">
         <v>375</v>
       </c>
@@ -41846,7 +41844,7 @@
       <c r="AL363" s="2"/>
       <c r="AM363" s="2"/>
     </row>
-    <row r="364" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A364" s="7" t="s">
         <v>376</v>
       </c>
@@ -41951,7 +41949,7 @@
       <c r="AL364" s="2"/>
       <c r="AM364" s="2"/>
     </row>
-    <row r="365" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A365" s="7" t="s">
         <v>377</v>
       </c>
@@ -42056,7 +42054,7 @@
       <c r="AL365" s="2"/>
       <c r="AM365" s="2"/>
     </row>
-    <row r="366" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A366" s="7" t="s">
         <v>378</v>
       </c>
@@ -42173,7 +42171,7 @@
         <v>7.1232876712328794E-2</v>
       </c>
     </row>
-    <row r="367" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A367" s="7" t="s">
         <v>379</v>
       </c>
@@ -42290,7 +42288,7 @@
         <v>7.1232876712328794E-2</v>
       </c>
     </row>
-    <row r="368" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A368" s="7" t="s">
         <v>428</v>
       </c>
@@ -42322,7 +42320,7 @@
       <c r="AL368" s="9"/>
       <c r="AM368" s="9"/>
     </row>
-    <row r="369" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A369" s="7" t="s">
         <v>429</v>
       </c>
@@ -42354,7 +42352,7 @@
       <c r="AL369" s="9"/>
       <c r="AM369" s="9"/>
     </row>
-    <row r="370" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A370" s="7" t="s">
         <v>430</v>
       </c>
@@ -42398,7 +42396,7 @@
         <v>5.1813471502590702E-3</v>
       </c>
     </row>
-    <row r="371" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A371" s="7" t="s">
         <v>431</v>
       </c>
@@ -42442,7 +42440,7 @@
         <v>5.1813471502590702E-3</v>
       </c>
     </row>
-    <row r="372" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A372" s="7" t="s">
         <v>432</v>
       </c>
@@ -42486,7 +42484,7 @@
         <v>0.34375</v>
       </c>
     </row>
-    <row r="373" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A373" s="7" t="s">
         <v>433</v>
       </c>
@@ -42531,13 +42529,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F373" xr:uid="{F1236420-0C1C-4AE2-B76E-36106E5A71DC}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="S"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -42550,13 +42541,13 @@
       <selection activeCell="F1" sqref="F1:AD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="54"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>2</v>
       </c>
@@ -42648,7 +42639,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
         <v>188</v>
       </c>
@@ -42740,7 +42731,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="60" t="s">
         <v>188</v>
       </c>
@@ -42829,7 +42820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="60" t="s">
         <v>188</v>
       </c>
@@ -42921,7 +42912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="60" t="s">
         <v>188</v>
       </c>
@@ -43013,7 +43004,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="60" t="s">
         <v>188</v>
       </c>
@@ -43105,7 +43096,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="60" t="s">
         <v>188</v>
       </c>
@@ -43197,7 +43188,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="60" t="s">
         <v>188</v>
       </c>
@@ -43289,7 +43280,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="66" t="s">
         <v>187</v>
       </c>
@@ -43381,7 +43372,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="66" t="s">
         <v>187</v>
       </c>
@@ -43473,7 +43464,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="66" t="s">
         <v>187</v>
       </c>
@@ -43565,7 +43556,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="66" t="s">
         <v>187</v>
       </c>
@@ -43657,7 +43648,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="66" t="s">
         <v>187</v>
       </c>
@@ -43749,7 +43740,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="66" t="s">
         <v>187</v>
       </c>
@@ -43841,7 +43832,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="67" t="s">
         <v>190</v>
       </c>
@@ -43933,7 +43924,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="67" t="s">
         <v>190</v>
       </c>
@@ -44025,7 +44016,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="67" t="s">
         <v>190</v>
       </c>
@@ -44117,7 +44108,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="18" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="67" t="s">
         <v>190</v>
       </c>
@@ -44209,7 +44200,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="67" t="s">
         <v>189</v>
       </c>
@@ -44301,7 +44292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="67" t="s">
         <v>189</v>
       </c>
@@ -44393,7 +44384,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="67" t="s">
         <v>189</v>
       </c>
@@ -44485,7 +44476,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="67" t="s">
         <v>189</v>
       </c>
@@ -44571,7 +44562,7 @@
       <c r="AC22" s="24"/>
       <c r="AD22" s="24"/>
     </row>
-    <row r="23" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="67" t="s">
         <v>197</v>
       </c>
@@ -44663,7 +44654,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="67" t="s">
         <v>197</v>
       </c>
@@ -44755,7 +44746,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="67" t="s">
         <v>195</v>
       </c>
@@ -44847,7 +44838,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="67" t="s">
         <v>195</v>
       </c>
@@ -44939,7 +44930,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="67" t="s">
         <v>195</v>
       </c>
@@ -45031,7 +45022,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="67" t="s">
         <v>198</v>
       </c>
@@ -45123,7 +45114,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="67" t="s">
         <v>198</v>
       </c>
@@ -45215,7 +45206,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="67" t="s">
         <v>196</v>
       </c>
@@ -45307,7 +45298,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="67" t="s">
         <v>196</v>
       </c>
@@ -45399,7 +45390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="67" t="s">
         <v>196</v>
       </c>
@@ -45491,7 +45482,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="33" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="67" t="s">
         <v>196</v>
       </c>
@@ -45583,7 +45574,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="34" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="67" t="s">
         <v>196</v>
       </c>
@@ -45686,18 +45677,18 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="54"/>
-    <col min="7" max="7" width="9.140625" style="9"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="54"/>
+    <col min="7" max="7" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
@@ -45742,7 +45733,7 @@
       <c r="T1" s="21"/>
       <c r="U1" s="55"/>
     </row>
-    <row r="2" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
         <v>446</v>
       </c>
@@ -45777,7 +45768,7 @@
         <v>0.176326375711575</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="54" t="s">
         <v>448</v>
       </c>
@@ -45812,7 +45803,7 @@
         <v>0.127184948857342</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="54" t="s">
         <v>449</v>
       </c>
@@ -45847,7 +45838,7 @@
         <v>0.16750096339113699</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="54" t="s">
         <v>446</v>
       </c>
@@ -45882,7 +45873,7 @@
         <v>0.110447817836812</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
         <v>448</v>
       </c>
@@ -45917,7 +45908,7 @@
         <v>3.8762711864406801E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="54" t="s">
         <v>449</v>
       </c>
@@ -45952,7 +45943,7 @@
         <v>0.13786042065009599</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
         <v>448</v>
       </c>
@@ -45987,7 +45978,7 @@
         <v>4.3557471264367799E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="54" t="s">
         <v>449</v>
       </c>
@@ -46022,7 +46013,7 @@
         <v>0.115406072106262</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="54" t="s">
         <v>446</v>
       </c>
@@ -46057,7 +46048,7 @@
         <v>0.13224791086351001</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
         <v>448</v>
       </c>
@@ -46092,7 +46083,7 @@
         <v>0.122546575800197</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>449</v>
       </c>
@@ -46127,7 +46118,7 @@
         <v>0.122561643835616</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="54" t="s">
         <v>446</v>
       </c>
@@ -46162,7 +46153,7 @@
         <v>4.8197771587743701E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="54" t="s">
         <v>448</v>
       </c>
@@ -46197,7 +46188,7 @@
         <v>2.6153424657534199E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="54" t="s">
         <v>449</v>
       </c>
@@ -46232,7 +46223,7 @@
         <v>7.1389041095890393E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="54" t="s">
         <v>446</v>
       </c>
@@ -46267,7 +46258,7 @@
         <v>1.1906976744186001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="54" t="s">
         <v>448</v>
       </c>
@@ -46302,7 +46293,7 @@
         <v>5.0906849315068503E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="54" t="s">
         <v>449</v>
       </c>
@@ -46337,7 +46328,7 @@
         <v>5.2484931506849297E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="54" t="s">
         <v>448</v>
       </c>
@@ -46366,7 +46357,7 @@
         <v>0.12214015151515201</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="54" t="s">
         <v>449</v>
       </c>
@@ -46395,7 +46386,7 @@
         <v>0.55826666666666602</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
         <v>448</v>
       </c>
@@ -46424,7 +46415,7 @@
         <v>0.10967803030303</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="54" t="s">
         <v>449</v>
       </c>
@@ -46453,7 +46444,7 @@
         <v>0.55407407407407405</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="54" t="s">
         <v>448</v>
       </c>
@@ -46482,7 +46473,7 @@
         <v>0.118661202185792</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="54" t="s">
         <v>449</v>
       </c>
@@ -46500,7 +46491,7 @@
       </c>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="54" t="s">
         <v>448</v>
       </c>
@@ -46529,7 +46520,7 @@
         <v>0.104781420765027</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="54" t="s">
         <v>449</v>
       </c>
@@ -46571,14 +46562,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -46589,7 +46580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>414</v>
       </c>
@@ -46600,7 +46591,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>416</v>
       </c>
@@ -46611,7 +46602,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>417</v>
       </c>
@@ -46622,7 +46613,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>415</v>
       </c>
@@ -46633,7 +46624,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>418</v>
       </c>
@@ -46644,7 +46635,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>419</v>
       </c>
@@ -46655,22 +46646,22 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>

</xml_diff>

<commit_message>
added soil physicochemical data for NPS feb samples
</commit_message>
<xml_diff>
--- a/data/met.xlsx
+++ b/data/met.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator/Documents/jaspreet/pico/pico_comb_run/pico/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9F366C-D99C-834F-A4BC-39289C6A0ED1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15760" yWindow="1440" windowWidth="32460" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1528,7 +1529,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1702,6 +1703,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Neutral 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
@@ -1987,8 +1994,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
-      <selection activeCell="E382" sqref="E382"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L376" sqref="L376:AE377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40557,6 +40565,66 @@
       <c r="K372" s="10" t="s">
         <v>428</v>
       </c>
+      <c r="L372" s="87">
+        <v>1.2</v>
+      </c>
+      <c r="M372" s="88">
+        <v>22</v>
+      </c>
+      <c r="N372" s="88">
+        <v>25</v>
+      </c>
+      <c r="O372" s="88">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P372" s="89">
+        <v>53</v>
+      </c>
+      <c r="Q372" s="89">
+        <v>88</v>
+      </c>
+      <c r="R372" s="89">
+        <v>526</v>
+      </c>
+      <c r="S372" s="89">
+        <v>55</v>
+      </c>
+      <c r="T372" s="88">
+        <v>6</v>
+      </c>
+      <c r="U372" s="88">
+        <v>6</v>
+      </c>
+      <c r="V372" s="88">
+        <v>12</v>
+      </c>
+      <c r="W372" s="88">
+        <v>13.2</v>
+      </c>
+      <c r="X372" s="88">
+        <v>15</v>
+      </c>
+      <c r="Y372" s="88">
+        <v>37</v>
+      </c>
+      <c r="Z372" s="87">
+        <v>0.7</v>
+      </c>
+      <c r="AA372" s="87">
+        <v>0.5</v>
+      </c>
+      <c r="AB372" s="87">
+        <v>0.2</v>
+      </c>
+      <c r="AC372" s="87">
+        <v>86</v>
+      </c>
+      <c r="AD372" s="87">
+        <v>6</v>
+      </c>
+      <c r="AE372" s="87">
+        <v>8</v>
+      </c>
       <c r="AF372" s="9"/>
       <c r="AG372" s="9"/>
       <c r="AH372" s="9"/>
@@ -40595,6 +40663,66 @@
       <c r="K373" s="10" t="s">
         <v>428</v>
       </c>
+      <c r="L373" s="87">
+        <v>1.2</v>
+      </c>
+      <c r="M373" s="88">
+        <v>22</v>
+      </c>
+      <c r="N373" s="88">
+        <v>25</v>
+      </c>
+      <c r="O373" s="88">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P373" s="89">
+        <v>53</v>
+      </c>
+      <c r="Q373" s="89">
+        <v>88</v>
+      </c>
+      <c r="R373" s="89">
+        <v>526</v>
+      </c>
+      <c r="S373" s="89">
+        <v>55</v>
+      </c>
+      <c r="T373" s="88">
+        <v>6</v>
+      </c>
+      <c r="U373" s="88">
+        <v>6</v>
+      </c>
+      <c r="V373" s="88">
+        <v>12</v>
+      </c>
+      <c r="W373" s="88">
+        <v>13.2</v>
+      </c>
+      <c r="X373" s="88">
+        <v>15</v>
+      </c>
+      <c r="Y373" s="88">
+        <v>37</v>
+      </c>
+      <c r="Z373" s="87">
+        <v>0.7</v>
+      </c>
+      <c r="AA373" s="87">
+        <v>0.5</v>
+      </c>
+      <c r="AB373" s="87">
+        <v>0.2</v>
+      </c>
+      <c r="AC373" s="87">
+        <v>86</v>
+      </c>
+      <c r="AD373" s="87">
+        <v>6</v>
+      </c>
+      <c r="AE373" s="87">
+        <v>8</v>
+      </c>
       <c r="AF373" s="9"/>
       <c r="AG373" s="9"/>
       <c r="AH373" s="9"/>
@@ -40633,6 +40761,66 @@
       <c r="K374" s="10" t="s">
         <v>428</v>
       </c>
+      <c r="L374" s="90">
+        <v>3.1</v>
+      </c>
+      <c r="M374" s="91">
+        <v>34</v>
+      </c>
+      <c r="N374" s="91">
+        <v>44</v>
+      </c>
+      <c r="O374" s="91">
+        <v>5.5</v>
+      </c>
+      <c r="P374" s="92">
+        <v>106.5</v>
+      </c>
+      <c r="Q374" s="92">
+        <v>110.5</v>
+      </c>
+      <c r="R374" s="92">
+        <v>477.5</v>
+      </c>
+      <c r="S374" s="92">
+        <v>72</v>
+      </c>
+      <c r="T374" s="91">
+        <v>4.8</v>
+      </c>
+      <c r="U374" s="91">
+        <v>9.5</v>
+      </c>
+      <c r="V374" s="91">
+        <v>4</v>
+      </c>
+      <c r="W374" s="91">
+        <v>23.4</v>
+      </c>
+      <c r="X374" s="91">
+        <v>26.5</v>
+      </c>
+      <c r="Y374" s="91">
+        <v>33</v>
+      </c>
+      <c r="Z374" s="90">
+        <v>1.05</v>
+      </c>
+      <c r="AA374" s="90">
+        <v>0.3</v>
+      </c>
+      <c r="AB374" s="90">
+        <v>0.1</v>
+      </c>
+      <c r="AC374" s="90">
+        <v>83.5</v>
+      </c>
+      <c r="AD374" s="90">
+        <v>7</v>
+      </c>
+      <c r="AE374" s="90">
+        <v>9.5</v>
+      </c>
       <c r="AF374" s="53">
         <v>17.601117948717899</v>
       </c>
@@ -40683,6 +40871,66 @@
       <c r="K375" s="10" t="s">
         <v>428</v>
       </c>
+      <c r="L375" s="90">
+        <v>3.1</v>
+      </c>
+      <c r="M375" s="91">
+        <v>34</v>
+      </c>
+      <c r="N375" s="91">
+        <v>44</v>
+      </c>
+      <c r="O375" s="91">
+        <v>5.5</v>
+      </c>
+      <c r="P375" s="92">
+        <v>106.5</v>
+      </c>
+      <c r="Q375" s="92">
+        <v>110.5</v>
+      </c>
+      <c r="R375" s="92">
+        <v>477.5</v>
+      </c>
+      <c r="S375" s="92">
+        <v>72</v>
+      </c>
+      <c r="T375" s="91">
+        <v>4.8</v>
+      </c>
+      <c r="U375" s="91">
+        <v>9.5</v>
+      </c>
+      <c r="V375" s="91">
+        <v>4</v>
+      </c>
+      <c r="W375" s="91">
+        <v>23.4</v>
+      </c>
+      <c r="X375" s="91">
+        <v>26.5</v>
+      </c>
+      <c r="Y375" s="91">
+        <v>33</v>
+      </c>
+      <c r="Z375" s="90">
+        <v>1.05</v>
+      </c>
+      <c r="AA375" s="90">
+        <v>0.3</v>
+      </c>
+      <c r="AB375" s="90">
+        <v>0.1</v>
+      </c>
+      <c r="AC375" s="90">
+        <v>83.5</v>
+      </c>
+      <c r="AD375" s="90">
+        <v>7</v>
+      </c>
+      <c r="AE375" s="90">
+        <v>9.5</v>
+      </c>
       <c r="AF375" s="53">
         <v>17.601117948717899</v>
       </c>
@@ -40733,6 +40981,66 @@
       <c r="K376" s="10" t="s">
         <v>428</v>
       </c>
+      <c r="L376" s="90">
+        <v>1.55</v>
+      </c>
+      <c r="M376" s="91">
+        <v>30</v>
+      </c>
+      <c r="N376" s="91">
+        <v>35</v>
+      </c>
+      <c r="O376" s="91">
+        <v>4.55</v>
+      </c>
+      <c r="P376" s="92">
+        <v>113</v>
+      </c>
+      <c r="Q376" s="92">
+        <v>76</v>
+      </c>
+      <c r="R376" s="92">
+        <v>235</v>
+      </c>
+      <c r="S376" s="92">
+        <v>66.5</v>
+      </c>
+      <c r="T376" s="91">
+        <v>5.4</v>
+      </c>
+      <c r="U376" s="91">
+        <v>7</v>
+      </c>
+      <c r="V376" s="91">
+        <v>5.85</v>
+      </c>
+      <c r="W376" s="91">
+        <v>17.5</v>
+      </c>
+      <c r="X376" s="91">
+        <v>9.25</v>
+      </c>
+      <c r="Y376" s="91">
+        <v>66.2</v>
+      </c>
+      <c r="Z376" s="90">
+        <v>0.4</v>
+      </c>
+      <c r="AA376" s="90">
+        <v>0.45</v>
+      </c>
+      <c r="AB376" s="90">
+        <v>0.2</v>
+      </c>
+      <c r="AC376" s="90">
+        <v>86</v>
+      </c>
+      <c r="AD376" s="90">
+        <v>4</v>
+      </c>
+      <c r="AE376" s="90">
+        <v>10</v>
+      </c>
       <c r="AF376" s="54">
         <v>14.345812499999999</v>
       </c>
@@ -40782,6 +41090,66 @@
       </c>
       <c r="K377" s="10" t="s">
         <v>428</v>
+      </c>
+      <c r="L377" s="90">
+        <v>1.55</v>
+      </c>
+      <c r="M377" s="91">
+        <v>30</v>
+      </c>
+      <c r="N377" s="91">
+        <v>35</v>
+      </c>
+      <c r="O377" s="91">
+        <v>4.55</v>
+      </c>
+      <c r="P377" s="92">
+        <v>113</v>
+      </c>
+      <c r="Q377" s="92">
+        <v>76</v>
+      </c>
+      <c r="R377" s="92">
+        <v>235</v>
+      </c>
+      <c r="S377" s="92">
+        <v>66.5</v>
+      </c>
+      <c r="T377" s="91">
+        <v>5.4</v>
+      </c>
+      <c r="U377" s="91">
+        <v>7</v>
+      </c>
+      <c r="V377" s="91">
+        <v>5.85</v>
+      </c>
+      <c r="W377" s="91">
+        <v>17.5</v>
+      </c>
+      <c r="X377" s="91">
+        <v>9.25</v>
+      </c>
+      <c r="Y377" s="91">
+        <v>66.2</v>
+      </c>
+      <c r="Z377" s="90">
+        <v>0.4</v>
+      </c>
+      <c r="AA377" s="90">
+        <v>0.45</v>
+      </c>
+      <c r="AB377" s="90">
+        <v>0.2</v>
+      </c>
+      <c r="AC377" s="90">
+        <v>86</v>
+      </c>
+      <c r="AD377" s="90">
+        <v>4</v>
+      </c>
+      <c r="AE377" s="90">
+        <v>10</v>
       </c>
       <c r="AF377" s="54">
         <v>14.345812499999999</v>

</xml_diff>